<commit_message>
update figures, output files
</commit_message>
<xml_diff>
--- a/clean-data/output/citizenship-norm-indicator-tables.xlsx
+++ b/clean-data/output/citizenship-norm-indicator-tables.xlsx
@@ -440,40 +440,40 @@
         <v>1999</v>
       </c>
       <c r="C2">
-        <v>0.9287573194534808</v>
+        <v>0.929</v>
       </c>
       <c r="D2">
-        <v>0.687035786630655</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="E2">
-        <v>0.7994714238519987</v>
+        <v>0.799</v>
       </c>
       <c r="F2">
-        <v>0.8806165956051164</v>
+        <v>0.881</v>
       </c>
       <c r="G2">
-        <v>0.7470647433747065</v>
+        <v>0.747</v>
       </c>
       <c r="H2">
-        <v>0.886208020867297</v>
+        <v>0.886</v>
       </c>
       <c r="I2">
-        <v>0.546538588936734</v>
+        <v>0.547</v>
       </c>
       <c r="J2">
-        <v>0.6673333333333333</v>
+        <v>0.667</v>
       </c>
       <c r="K2">
-        <v>0.5040053404539386</v>
+        <v>0.504</v>
       </c>
       <c r="L2">
-        <v>0.5771954674220963</v>
+        <v>0.577</v>
       </c>
       <c r="M2">
-        <v>0.3389423076923077</v>
+        <v>0.339</v>
       </c>
       <c r="N2">
-        <v>0.1739424703891709</v>
+        <v>0.174</v>
       </c>
     </row>
     <row r="3">
@@ -486,40 +486,40 @@
         <v>2009</v>
       </c>
       <c r="C3">
-        <v>0.8398072869617585</v>
+        <v>0.84</v>
       </c>
       <c r="D3">
-        <v>0.7592033796016898</v>
+        <v>0.759</v>
       </c>
       <c r="E3">
-        <v>0.7545289855072463</v>
+        <v>0.755</v>
       </c>
       <c r="F3">
-        <v>0.6304347826086957</v>
+        <v>0.63</v>
       </c>
       <c r="G3">
-        <v>0.6721954161640531</v>
+        <v>0.672</v>
       </c>
       <c r="H3">
-        <v>0.734375</v>
+        <v>0.734</v>
       </c>
       <c r="I3">
-        <v>0.7719298245614035</v>
+        <v>0.772</v>
       </c>
       <c r="J3">
-        <v>0.6792509815765629</v>
+        <v>0.679</v>
       </c>
       <c r="K3">
-        <v>0.6869722557297949</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="L3">
-        <v>0.6140138930836605</v>
+        <v>0.614</v>
       </c>
       <c r="M3">
-        <v>0.3621523579201935</v>
+        <v>0.362</v>
       </c>
       <c r="N3">
-        <v>0.2765700483091788</v>
+        <v>0.277</v>
       </c>
     </row>
     <row r="4">
@@ -532,40 +532,40 @@
         <v>2009</v>
       </c>
       <c r="C4">
-        <v>0.8709239130434783</v>
+        <v>0.871</v>
       </c>
       <c r="D4">
-        <v>0.7703300442327322</v>
+        <v>0.77</v>
       </c>
       <c r="E4">
-        <v>0.7649659863945578</v>
+        <v>0.765</v>
       </c>
       <c r="F4">
-        <v>0.7756279701289884</v>
+        <v>0.776</v>
       </c>
       <c r="G4">
-        <v>0.7907608695652174</v>
+        <v>0.791</v>
       </c>
       <c r="H4">
-        <v>0.8203998644527278</v>
+        <v>0.82</v>
       </c>
       <c r="I4">
-        <v>0.4652588555858311</v>
+        <v>0.465</v>
       </c>
       <c r="J4">
-        <v>0.8242876526458616</v>
+        <v>0.824</v>
       </c>
       <c r="K4">
-        <v>0.6571815718157181</v>
+        <v>0.657</v>
       </c>
       <c r="L4">
-        <v>0.4577249575551783</v>
+        <v>0.458</v>
       </c>
       <c r="M4">
-        <v>0.313179347826087</v>
+        <v>0.313</v>
       </c>
       <c r="N4">
-        <v>0.1572348356489326</v>
+        <v>0.157</v>
       </c>
     </row>
     <row r="5">
@@ -578,40 +578,40 @@
         <v>2016</v>
       </c>
       <c r="C5">
-        <v>0.9343015214384509</v>
+        <v>0.9340000000000001</v>
       </c>
       <c r="D5">
-        <v>0.8141379310344827</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="E5">
-        <v>0.8035220994475138</v>
+        <v>0.804</v>
       </c>
       <c r="F5">
-        <v>0.8631034482758621</v>
+        <v>0.863</v>
       </c>
       <c r="G5">
-        <v>0.8645473393227368</v>
+        <v>0.865</v>
       </c>
       <c r="H5">
-        <v>0.8457574716592237</v>
+        <v>0.846</v>
       </c>
       <c r="I5">
-        <v>0.5680718728403593</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="J5">
-        <v>0.8785271851342051</v>
+        <v>0.879</v>
       </c>
       <c r="K5">
-        <v>0.7107438016528925</v>
+        <v>0.711</v>
       </c>
       <c r="L5">
-        <v>0.4960193838698512</v>
+        <v>0.496</v>
       </c>
       <c r="M5">
-        <v>0.3777239709443099</v>
+        <v>0.378</v>
       </c>
       <c r="N5">
-        <v>0.1596292481977343</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="6">
@@ -624,40 +624,40 @@
         <v>1999</v>
       </c>
       <c r="C6">
-        <v>0.9063765182186235</v>
+        <v>0.906</v>
       </c>
       <c r="D6">
-        <v>0.776464542651593</v>
+        <v>0.776</v>
       </c>
       <c r="E6">
-        <v>0.5622406639004149</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="F6">
-        <v>0.5403598971722365</v>
+        <v>0.54</v>
       </c>
       <c r="G6">
-        <v>0.7199587416193914</v>
+        <v>0.72</v>
       </c>
       <c r="H6">
-        <v>0.8148893360160966</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="I6">
-        <v>0.4187817258883249</v>
+        <v>0.419</v>
       </c>
       <c r="J6">
-        <v>0.5545502927088877</v>
+        <v>0.555</v>
       </c>
       <c r="K6">
-        <v>0.5787863335033147</v>
+        <v>0.579</v>
       </c>
       <c r="L6">
-        <v>0.5635478637101136</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="M6">
-        <v>0.3865284974093264</v>
+        <v>0.387</v>
       </c>
       <c r="N6">
-        <v>0.2243723849372385</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="7">
@@ -670,40 +670,40 @@
         <v>1999</v>
       </c>
       <c r="C7">
-        <v>0.8667903525046382</v>
+        <v>0.867</v>
       </c>
       <c r="D7">
-        <v>0.8225058004640371</v>
+        <v>0.823</v>
       </c>
       <c r="E7">
-        <v>0.6767757382282522</v>
+        <v>0.677</v>
       </c>
       <c r="F7">
-        <v>0.8159392789373814</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G7">
-        <v>0.8146703082325399</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="H7">
-        <v>0.7074202229911573</v>
+        <v>0.707</v>
       </c>
       <c r="I7">
-        <v>0.7993791230112534</v>
+        <v>0.799</v>
       </c>
       <c r="J7">
-        <v>0.6759404388714734</v>
+        <v>0.676</v>
       </c>
       <c r="K7">
-        <v>0.6757797458606084</v>
+        <v>0.676</v>
       </c>
       <c r="L7">
-        <v>0.708992506244796</v>
+        <v>0.709</v>
       </c>
       <c r="M7">
-        <v>0.4818976279650437</v>
+        <v>0.482</v>
       </c>
       <c r="N7">
-        <v>0.3926482873851295</v>
+        <v>0.393</v>
       </c>
     </row>
     <row r="8">
@@ -716,40 +716,40 @@
         <v>2009</v>
       </c>
       <c r="C8">
-        <v>0.8483788938334393</v>
+        <v>0.848</v>
       </c>
       <c r="D8">
-        <v>0.9029064196742255</v>
+        <v>0.903</v>
       </c>
       <c r="E8">
-        <v>0.8689413265306123</v>
+        <v>0.869</v>
       </c>
       <c r="F8">
-        <v>0.8885705189430118</v>
+        <v>0.889</v>
       </c>
       <c r="G8">
-        <v>0.8966177409061902</v>
+        <v>0.897</v>
       </c>
       <c r="H8">
-        <v>0.6876971608832808</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="I8">
-        <v>0.8531379420197515</v>
+        <v>0.853</v>
       </c>
       <c r="J8">
-        <v>0.6747371774450462</v>
+        <v>0.675</v>
       </c>
       <c r="K8">
-        <v>0.6492845786963434</v>
+        <v>0.649</v>
       </c>
       <c r="L8">
-        <v>0.7300672430355427</v>
+        <v>0.73</v>
       </c>
       <c r="M8">
-        <v>0.3455128205128205</v>
+        <v>0.346</v>
       </c>
       <c r="N8">
-        <v>0.2048919949174079</v>
+        <v>0.205</v>
       </c>
     </row>
     <row r="9">
@@ -762,40 +762,40 @@
         <v>2016</v>
       </c>
       <c r="C9">
-        <v>0.8366561734872333</v>
+        <v>0.837</v>
       </c>
       <c r="D9">
-        <v>0.9015597920277296</v>
+        <v>0.902</v>
       </c>
       <c r="E9">
-        <v>0.8735314443676572</v>
+        <v>0.874</v>
       </c>
       <c r="F9">
-        <v>0.8941707147814018</v>
+        <v>0.894</v>
       </c>
       <c r="G9">
-        <v>0.9038861901457321</v>
+        <v>0.904</v>
       </c>
       <c r="H9">
-        <v>0.7594631796283551</v>
+        <v>0.759</v>
       </c>
       <c r="I9">
-        <v>0.8880778588807786</v>
+        <v>0.888</v>
       </c>
       <c r="J9">
-        <v>0.723050259965338</v>
+        <v>0.723</v>
       </c>
       <c r="K9">
-        <v>0.6394064872325742</v>
+        <v>0.639</v>
       </c>
       <c r="L9">
-        <v>0.7603048146865258</v>
+        <v>0.76</v>
       </c>
       <c r="M9">
-        <v>0.3681453021306322</v>
+        <v>0.368</v>
       </c>
       <c r="N9">
-        <v>0.2313278008298755</v>
+        <v>0.231</v>
       </c>
     </row>
     <row r="10">
@@ -808,40 +808,40 @@
         <v>1999</v>
       </c>
       <c r="C10">
-        <v>0.9543363994743759</v>
+        <v>0.954</v>
       </c>
       <c r="D10">
-        <v>0.8769334229993275</v>
+        <v>0.877</v>
       </c>
       <c r="E10">
-        <v>0.7631578947368421</v>
+        <v>0.763</v>
       </c>
       <c r="F10">
-        <v>0.6670064559972817</v>
+        <v>0.667</v>
       </c>
       <c r="G10">
-        <v>0.6986531986531986</v>
+        <v>0.699</v>
       </c>
       <c r="H10">
-        <v>0.685799601857996</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="I10">
-        <v>0.6230331436223636</v>
+        <v>0.623</v>
       </c>
       <c r="J10">
-        <v>0.7306079664570231</v>
+        <v>0.731</v>
       </c>
       <c r="K10">
-        <v>0.7525569119102606</v>
+        <v>0.753</v>
       </c>
       <c r="L10">
-        <v>0.6271604938271605</v>
+        <v>0.627</v>
       </c>
       <c r="M10">
-        <v>0.4236134739707383</v>
+        <v>0.424</v>
       </c>
       <c r="N10">
-        <v>0.2349914236706689</v>
+        <v>0.235</v>
       </c>
     </row>
     <row r="11">
@@ -854,40 +854,40 @@
         <v>2009</v>
       </c>
       <c r="C11">
-        <v>0.8852686308492201</v>
+        <v>0.885</v>
       </c>
       <c r="D11">
-        <v>0.7328695652173913</v>
+        <v>0.733</v>
       </c>
       <c r="E11">
-        <v>0.6455210874869293</v>
+        <v>0.646</v>
       </c>
       <c r="F11">
-        <v>0.6738227146814404</v>
+        <v>0.674</v>
       </c>
       <c r="G11">
-        <v>0.7133448873483536</v>
+        <v>0.713</v>
       </c>
       <c r="H11">
-        <v>0.7164539496378062</v>
+        <v>0.716</v>
       </c>
       <c r="I11">
-        <v>0.7409722222222223</v>
+        <v>0.741</v>
       </c>
       <c r="J11">
-        <v>0.7966747488742639</v>
+        <v>0.797</v>
       </c>
       <c r="K11">
-        <v>0.7461139896373057</v>
+        <v>0.746</v>
       </c>
       <c r="L11">
-        <v>0.5076495132127955</v>
+        <v>0.508</v>
       </c>
       <c r="M11">
-        <v>0.3642980935875217</v>
+        <v>0.364</v>
       </c>
       <c r="N11">
-        <v>0.2957063711911357</v>
+        <v>0.296</v>
       </c>
     </row>
     <row r="12">
@@ -900,40 +900,40 @@
         <v>1999</v>
       </c>
       <c r="C12">
-        <v>0.9536101083032491</v>
+        <v>0.954</v>
       </c>
       <c r="D12">
-        <v>0.8259359320725589</v>
+        <v>0.826</v>
       </c>
       <c r="E12">
-        <v>0.8842719154364862</v>
+        <v>0.884</v>
       </c>
       <c r="F12">
-        <v>0.8665441176470589</v>
+        <v>0.867</v>
       </c>
       <c r="G12">
-        <v>0.8908661703286725</v>
+        <v>0.891</v>
       </c>
       <c r="H12">
-        <v>0.9103722443079147</v>
+        <v>0.91</v>
       </c>
       <c r="I12">
-        <v>0.8759272997032641</v>
+        <v>0.876</v>
       </c>
       <c r="J12">
-        <v>0.8568522285925652</v>
+        <v>0.857</v>
       </c>
       <c r="K12">
-        <v>0.7962359753890699</v>
+        <v>0.796</v>
       </c>
       <c r="L12">
-        <v>0.6163928012519562</v>
+        <v>0.616</v>
       </c>
       <c r="M12">
-        <v>0.3450360834796177</v>
+        <v>0.345</v>
       </c>
       <c r="N12">
-        <v>0.4385491028361952</v>
+        <v>0.439</v>
       </c>
     </row>
     <row r="13">
@@ -946,40 +946,40 @@
         <v>2009</v>
       </c>
       <c r="C13">
-        <v>0.889192352711666</v>
+        <v>0.889</v>
       </c>
       <c r="D13">
-        <v>0.8838482596793117</v>
+        <v>0.884</v>
       </c>
       <c r="E13">
-        <v>0.9030243902439025</v>
+        <v>0.903</v>
       </c>
       <c r="F13">
-        <v>0.8043222003929273</v>
+        <v>0.804</v>
       </c>
       <c r="G13">
-        <v>0.9025821596244131</v>
+        <v>0.903</v>
       </c>
       <c r="H13">
-        <v>0.8281827016520894</v>
+        <v>0.828</v>
       </c>
       <c r="I13">
-        <v>0.8514599255339996</v>
+        <v>0.851</v>
       </c>
       <c r="J13">
-        <v>0.8489278752436648</v>
+        <v>0.849</v>
       </c>
       <c r="K13">
-        <v>0.6773500097713504</v>
+        <v>0.677</v>
       </c>
       <c r="L13">
-        <v>0.6610666145731589</v>
+        <v>0.661</v>
       </c>
       <c r="M13">
-        <v>0.2981257321358844</v>
+        <v>0.298</v>
       </c>
       <c r="N13">
-        <v>0.2998243216865118</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="14">
@@ -992,40 +992,40 @@
         <v>2016</v>
       </c>
       <c r="C14">
-        <v>0.8760529482551144</v>
+        <v>0.876</v>
       </c>
       <c r="D14">
-        <v>0.8390920048212134</v>
+        <v>0.839</v>
       </c>
       <c r="E14">
-        <v>0.8386773547094188</v>
+        <v>0.839</v>
       </c>
       <c r="F14">
-        <v>0.7789197904070939</v>
+        <v>0.779</v>
       </c>
       <c r="G14">
-        <v>0.8618130766145207</v>
+        <v>0.862</v>
       </c>
       <c r="H14">
-        <v>0.7805316809914051</v>
+        <v>0.781</v>
       </c>
       <c r="I14">
-        <v>0.8311244979919679</v>
+        <v>0.831</v>
       </c>
       <c r="J14">
-        <v>0.7665533106621324</v>
+        <v>0.767</v>
       </c>
       <c r="K14">
-        <v>0.6502699460107978</v>
+        <v>0.65</v>
       </c>
       <c r="L14">
-        <v>0.6646610509426394</v>
+        <v>0.665</v>
       </c>
       <c r="M14">
-        <v>0.4201444622792938</v>
+        <v>0.42</v>
       </c>
       <c r="N14">
-        <v>0.3485485485485486</v>
+        <v>0.349</v>
       </c>
     </row>
     <row r="15">
@@ -1038,40 +1038,40 @@
         <v>1999</v>
       </c>
       <c r="C15">
-        <v>0.9737226277372263</v>
+        <v>0.974</v>
       </c>
       <c r="D15">
-        <v>0.9408347676419966</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="E15">
-        <v>0.9420320404721754</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="F15">
-        <v>0.8372605153049989</v>
+        <v>0.837</v>
       </c>
       <c r="G15">
-        <v>0.9392670157068063</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="H15">
-        <v>0.8791631084543126</v>
+        <v>0.879</v>
       </c>
       <c r="I15">
-        <v>0.8427437141596824</v>
+        <v>0.843</v>
       </c>
       <c r="J15">
-        <v>0.861832224844454</v>
+        <v>0.862</v>
       </c>
       <c r="K15">
-        <v>0.6615143369175627</v>
+        <v>0.662</v>
       </c>
       <c r="L15">
-        <v>0.8071099407504937</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="M15">
-        <v>0.5129083847384053</v>
+        <v>0.513</v>
       </c>
       <c r="N15">
-        <v>0.577250748330647</v>
+        <v>0.577</v>
       </c>
     </row>
     <row r="16">
@@ -1084,40 +1084,40 @@
         <v>2009</v>
       </c>
       <c r="C16">
-        <v>0.8751907749703239</v>
+        <v>0.875</v>
       </c>
       <c r="D16">
-        <v>0.9412559081701553</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="E16">
-        <v>0.8983767331755157</v>
+        <v>0.898</v>
       </c>
       <c r="F16">
-        <v>0.8112244897959183</v>
+        <v>0.8110000000000001</v>
       </c>
       <c r="G16">
-        <v>0.9603120759837178</v>
+        <v>0.96</v>
       </c>
       <c r="H16">
-        <v>0.8706666666666667</v>
+        <v>0.871</v>
       </c>
       <c r="I16">
-        <v>0.8903478854024557</v>
+        <v>0.89</v>
       </c>
       <c r="J16">
-        <v>0.8545669025952141</v>
+        <v>0.855</v>
       </c>
       <c r="K16">
-        <v>0.6444594366672288</v>
+        <v>0.644</v>
       </c>
       <c r="L16">
-        <v>0.7054118447923757</v>
+        <v>0.705</v>
       </c>
       <c r="M16">
-        <v>0.2924640135478408</v>
+        <v>0.292</v>
       </c>
       <c r="N16">
-        <v>0.31993921998987</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="17">
@@ -1130,40 +1130,40 @@
         <v>2016</v>
       </c>
       <c r="C17">
-        <v>0.8921385991058122</v>
+        <v>0.892</v>
       </c>
       <c r="D17">
-        <v>0.9250832408435072</v>
+        <v>0.925</v>
       </c>
       <c r="E17">
-        <v>0.8835095529586348</v>
+        <v>0.884</v>
       </c>
       <c r="F17">
-        <v>0.8220291997782295</v>
+        <v>0.822</v>
       </c>
       <c r="G17">
-        <v>0.9513143280266568</v>
+        <v>0.951</v>
       </c>
       <c r="H17">
-        <v>0.8454097463040701</v>
+        <v>0.845</v>
       </c>
       <c r="I17">
-        <v>0.901193139448173</v>
+        <v>0.901</v>
       </c>
       <c r="J17">
-        <v>0.8354617804923191</v>
+        <v>0.835</v>
       </c>
       <c r="K17">
-        <v>0.6575796647633082</v>
+        <v>0.658</v>
       </c>
       <c r="L17">
-        <v>0.7051424343322235</v>
+        <v>0.705</v>
       </c>
       <c r="M17">
-        <v>0.3204225352112676</v>
+        <v>0.32</v>
       </c>
       <c r="N17">
-        <v>0.3024884792626728</v>
+        <v>0.302</v>
       </c>
     </row>
     <row r="18">
@@ -1176,40 +1176,40 @@
         <v>1999</v>
       </c>
       <c r="C18">
-        <v>0.9739498534679257</v>
+        <v>0.974</v>
       </c>
       <c r="D18">
-        <v>0.9372948128693368</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="E18">
-        <v>0.9148450244698205</v>
+        <v>0.915</v>
       </c>
       <c r="F18">
-        <v>0.6816976127320955</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="G18">
-        <v>0.7931825630940675</v>
+        <v>0.793</v>
       </c>
       <c r="H18">
-        <v>0.9135152910226899</v>
+        <v>0.914</v>
       </c>
       <c r="I18">
-        <v>0.9256360078277887</v>
+        <v>0.926</v>
       </c>
       <c r="J18">
-        <v>0.9088808187520634</v>
+        <v>0.909</v>
       </c>
       <c r="K18">
-        <v>0.8600392413342054</v>
+        <v>0.86</v>
       </c>
       <c r="L18">
-        <v>0.8521008403361344</v>
+        <v>0.852</v>
       </c>
       <c r="M18">
-        <v>0.5591000671591673</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="N18">
-        <v>0.4752176825184193</v>
+        <v>0.475</v>
       </c>
     </row>
     <row r="19">
@@ -1222,40 +1222,40 @@
         <v>2009</v>
       </c>
       <c r="C19">
-        <v>0.8108816781383154</v>
+        <v>0.8110000000000001</v>
       </c>
       <c r="D19">
-        <v>0.837471036080768</v>
+        <v>0.837</v>
       </c>
       <c r="E19">
-        <v>0.7462834489593657</v>
+        <v>0.746</v>
       </c>
       <c r="F19">
-        <v>0.7179993418887792</v>
+        <v>0.718</v>
       </c>
       <c r="G19">
-        <v>0.8050875454245128</v>
+        <v>0.805</v>
       </c>
       <c r="H19">
-        <v>0.8208809135399674</v>
+        <v>0.821</v>
       </c>
       <c r="I19">
-        <v>0.8323985483338832</v>
+        <v>0.832</v>
       </c>
       <c r="J19">
-        <v>0.7935779816513762</v>
+        <v>0.794</v>
       </c>
       <c r="K19">
-        <v>0.7077326343381389</v>
+        <v>0.708</v>
       </c>
       <c r="L19">
-        <v>0.7493421052631579</v>
+        <v>0.749</v>
       </c>
       <c r="M19">
-        <v>0.5858085808580858</v>
+        <v>0.586</v>
       </c>
       <c r="N19">
-        <v>0.4654211733857752</v>
+        <v>0.465</v>
       </c>
     </row>
     <row r="20">
@@ -1268,40 +1268,40 @@
         <v>1999</v>
       </c>
       <c r="C20">
-        <v>0.9739568748249789</v>
+        <v>0.974</v>
       </c>
       <c r="D20">
-        <v>0.8229433532593226</v>
+        <v>0.823</v>
       </c>
       <c r="E20">
-        <v>0.7886963930701505</v>
+        <v>0.789</v>
       </c>
       <c r="F20">
-        <v>0.7724550898203593</v>
+        <v>0.772</v>
       </c>
       <c r="G20">
-        <v>0.8161081385525204</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="H20">
-        <v>0.6797863368006747</v>
+        <v>0.68</v>
       </c>
       <c r="I20">
-        <v>0.7157775896133221</v>
+        <v>0.716</v>
       </c>
       <c r="J20">
-        <v>0.4272543935465284</v>
+        <v>0.427</v>
       </c>
       <c r="K20">
-        <v>0.7276035834266518</v>
+        <v>0.728</v>
       </c>
       <c r="L20">
-        <v>0.670487948265726</v>
+        <v>0.67</v>
       </c>
       <c r="M20">
-        <v>0.28125</v>
+        <v>0.281</v>
       </c>
       <c r="N20">
-        <v>0.1356667630893839</v>
+        <v>0.136</v>
       </c>
     </row>
     <row r="21">
@@ -1314,40 +1314,40 @@
         <v>2009</v>
       </c>
       <c r="C21">
-        <v>0.9219565217391305</v>
+        <v>0.922</v>
       </c>
       <c r="D21">
-        <v>0.8167287059338735</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="E21">
-        <v>0.7668348322000439</v>
+        <v>0.767</v>
       </c>
       <c r="F21">
-        <v>0.95119825708061</v>
+        <v>0.951</v>
       </c>
       <c r="G21">
-        <v>0.8348282651498578</v>
+        <v>0.835</v>
       </c>
       <c r="H21">
-        <v>0.6829533116178067</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="I21">
-        <v>0.6449781659388646</v>
+        <v>0.645</v>
       </c>
       <c r="J21">
-        <v>0.4582697755502288</v>
+        <v>0.458</v>
       </c>
       <c r="K21">
-        <v>0.6574417084332098</v>
+        <v>0.657</v>
       </c>
       <c r="L21">
-        <v>0.5429696041985568</v>
+        <v>0.543</v>
       </c>
       <c r="M21">
-        <v>0.3476460331299041</v>
+        <v>0.348</v>
       </c>
       <c r="N21">
-        <v>0.1507296885210194</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="22">
@@ -1360,40 +1360,40 @@
         <v>1999</v>
       </c>
       <c r="C22">
-        <v>0.9478791239257001</v>
+        <v>0.948</v>
       </c>
       <c r="D22">
-        <v>0.902010761823846</v>
+        <v>0.902</v>
       </c>
       <c r="E22">
-        <v>0.8421201014942205</v>
+        <v>0.842</v>
       </c>
       <c r="F22">
-        <v>0.6601857225769008</v>
+        <v>0.66</v>
       </c>
       <c r="G22">
-        <v>0.7166904422253922</v>
+        <v>0.717</v>
       </c>
       <c r="H22">
-        <v>0.6974015088013411</v>
+        <v>0.697</v>
       </c>
       <c r="I22">
-        <v>0.5846681922196796</v>
+        <v>0.585</v>
       </c>
       <c r="J22">
-        <v>0.6880415944540728</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="K22">
-        <v>0.7032167832167833</v>
+        <v>0.703</v>
       </c>
       <c r="L22">
-        <v>0.6850299401197605</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="M22">
-        <v>0.4328401508558167</v>
+        <v>0.433</v>
       </c>
       <c r="N22">
-        <v>0.1857394366197183</v>
+        <v>0.186</v>
       </c>
     </row>
     <row r="23">
@@ -1406,40 +1406,40 @@
         <v>1999</v>
       </c>
       <c r="C23">
-        <v>0.9514781491002571</v>
+        <v>0.951</v>
       </c>
       <c r="D23">
-        <v>0.7860851505711319</v>
+        <v>0.786</v>
       </c>
       <c r="E23">
-        <v>0.8640552995391705</v>
+        <v>0.864</v>
       </c>
       <c r="F23">
-        <v>0.5943869027731373</v>
+        <v>0.594</v>
       </c>
       <c r="G23">
-        <v>0.8232558139534883</v>
+        <v>0.823</v>
       </c>
       <c r="H23">
-        <v>0.6075949367088608</v>
+        <v>0.608</v>
       </c>
       <c r="I23">
-        <v>0.4453560879553659</v>
+        <v>0.445</v>
       </c>
       <c r="J23">
-        <v>0.6311447232726023</v>
+        <v>0.631</v>
       </c>
       <c r="K23">
-        <v>0.6703800786369594</v>
+        <v>0.67</v>
       </c>
       <c r="L23">
-        <v>0.5353241077931536</v>
+        <v>0.535</v>
       </c>
       <c r="M23">
-        <v>0.4418194640338505</v>
+        <v>0.442</v>
       </c>
       <c r="N23">
-        <v>0.1715353260869565</v>
+        <v>0.172</v>
       </c>
     </row>
     <row r="24">
@@ -1452,40 +1452,40 @@
         <v>2009</v>
       </c>
       <c r="C24">
-        <v>0.943002780352178</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="D24">
-        <v>0.6881545264137771</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="E24">
-        <v>0.5543884220354809</v>
+        <v>0.554</v>
       </c>
       <c r="F24">
-        <v>0.7497674418604651</v>
+        <v>0.75</v>
       </c>
       <c r="G24">
-        <v>0.7629990714948932</v>
+        <v>0.763</v>
       </c>
       <c r="H24">
-        <v>0.7908210332103321</v>
+        <v>0.791</v>
       </c>
       <c r="I24">
-        <v>0.6774118738404453</v>
+        <v>0.677</v>
       </c>
       <c r="J24">
-        <v>0.8826258408721874</v>
+        <v>0.883</v>
       </c>
       <c r="K24">
-        <v>0.7760296159185562</v>
+        <v>0.776</v>
       </c>
       <c r="L24">
-        <v>0.4191672481972551</v>
+        <v>0.419</v>
       </c>
       <c r="M24">
-        <v>0.2552747507535358</v>
+        <v>0.255</v>
       </c>
       <c r="N24">
-        <v>0.2153098982423682</v>
+        <v>0.215</v>
       </c>
     </row>
     <row r="25">
@@ -1498,40 +1498,40 @@
         <v>2016</v>
       </c>
       <c r="C25">
-        <v>0.9507480248781308</v>
+        <v>0.951</v>
       </c>
       <c r="D25">
-        <v>0.7132973337833277</v>
+        <v>0.713</v>
       </c>
       <c r="E25">
-        <v>0.5735269289211549</v>
+        <v>0.574</v>
       </c>
       <c r="F25">
-        <v>0.8538513286242853</v>
+        <v>0.854</v>
       </c>
       <c r="G25">
-        <v>0.7291736930860033</v>
+        <v>0.729</v>
       </c>
       <c r="H25">
-        <v>0.88107202680067</v>
+        <v>0.881</v>
       </c>
       <c r="I25">
-        <v>0.7618807724601175</v>
+        <v>0.762</v>
       </c>
       <c r="J25">
-        <v>0.9210614712798119</v>
+        <v>0.921</v>
       </c>
       <c r="K25">
-        <v>0.8226510067114094</v>
+        <v>0.823</v>
       </c>
       <c r="L25">
-        <v>0.4120518431240532</v>
+        <v>0.412</v>
       </c>
       <c r="M25">
-        <v>0.3116271243479724</v>
+        <v>0.312</v>
       </c>
       <c r="N25">
-        <v>0.2295412535708284</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="26">
@@ -1544,40 +1544,40 @@
         <v>2016</v>
       </c>
       <c r="C26">
-        <v>0.9501754385964912</v>
+        <v>0.95</v>
       </c>
       <c r="D26">
-        <v>0.8787666433076384</v>
+        <v>0.879</v>
       </c>
       <c r="E26">
-        <v>0.798728813559322</v>
+        <v>0.799</v>
       </c>
       <c r="F26">
-        <v>0.6311360448807855</v>
+        <v>0.631</v>
       </c>
       <c r="G26">
-        <v>0.6713780918727915</v>
+        <v>0.671</v>
       </c>
       <c r="H26">
-        <v>0.6592022393282015</v>
+        <v>0.659</v>
       </c>
       <c r="I26">
-        <v>0.7291371994342292</v>
+        <v>0.729</v>
       </c>
       <c r="J26">
-        <v>0.8335674157303371</v>
+        <v>0.834</v>
       </c>
       <c r="K26">
-        <v>0.7700908455625437</v>
+        <v>0.77</v>
       </c>
       <c r="L26">
-        <v>0.5400280898876404</v>
+        <v>0.54</v>
       </c>
       <c r="M26">
-        <v>0.3494397759103641</v>
+        <v>0.349</v>
       </c>
       <c r="N26">
-        <v>0.1635220125786163</v>
+        <v>0.164</v>
       </c>
     </row>
     <row r="27">
@@ -1590,40 +1590,40 @@
         <v>2009</v>
       </c>
       <c r="C27">
-        <v>0.9130783631987163</v>
+        <v>0.913</v>
       </c>
       <c r="D27">
-        <v>0.906572514937534</v>
+        <v>0.907</v>
       </c>
       <c r="E27">
-        <v>0.8398373983739837</v>
+        <v>0.84</v>
       </c>
       <c r="F27">
-        <v>0.9073672806067172</v>
+        <v>0.907</v>
       </c>
       <c r="G27">
-        <v>0.9252107696491705</v>
+        <v>0.925</v>
       </c>
       <c r="H27">
-        <v>0.812199443178942</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="I27">
-        <v>0.9237196765498652</v>
+        <v>0.924</v>
       </c>
       <c r="J27">
-        <v>0.8738714816781731</v>
+        <v>0.874</v>
       </c>
       <c r="K27">
-        <v>0.7733191602444858</v>
+        <v>0.773</v>
       </c>
       <c r="L27">
-        <v>0.6834115373999448</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="M27">
-        <v>0.3217107055298284</v>
+        <v>0.322</v>
       </c>
       <c r="N27">
-        <v>0.5885623510722796</v>
+        <v>0.589</v>
       </c>
     </row>
     <row r="28">
@@ -1636,40 +1636,40 @@
         <v>2016</v>
       </c>
       <c r="C28">
-        <v>0.9385813148788927</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="D28">
-        <v>0.9194572748267898</v>
+        <v>0.919</v>
       </c>
       <c r="E28">
-        <v>0.8915420023014959</v>
+        <v>0.892</v>
       </c>
       <c r="F28">
-        <v>0.9252873563218391</v>
+        <v>0.925</v>
       </c>
       <c r="G28">
-        <v>0.9514871498700549</v>
+        <v>0.951</v>
       </c>
       <c r="H28">
-        <v>0.7702589807852965</v>
+        <v>0.77</v>
       </c>
       <c r="I28">
-        <v>0.9425725168473483</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="J28">
-        <v>0.916261789082595</v>
+        <v>0.916</v>
       </c>
       <c r="K28">
-        <v>0.8358671171171171</v>
+        <v>0.836</v>
       </c>
       <c r="L28">
-        <v>0.7259643062751872</v>
+        <v>0.726</v>
       </c>
       <c r="M28">
-        <v>0.3893549320219844</v>
+        <v>0.389</v>
       </c>
       <c r="N28">
-        <v>0.5888888888888889</v>
+        <v>0.589</v>
       </c>
     </row>
     <row r="29">
@@ -1682,40 +1682,40 @@
         <v>1999</v>
       </c>
       <c r="C29">
-        <v>0.9744218640504555</v>
+        <v>0.974</v>
       </c>
       <c r="D29">
-        <v>0.7206044968669369</v>
+        <v>0.721</v>
       </c>
       <c r="E29">
-        <v>0.784862043251305</v>
+        <v>0.785</v>
       </c>
       <c r="F29">
-        <v>0.9266642933428266</v>
+        <v>0.927</v>
       </c>
       <c r="G29">
-        <v>0.7634566093006225</v>
+        <v>0.763</v>
       </c>
       <c r="H29">
-        <v>0.7602982954545454</v>
+        <v>0.76</v>
       </c>
       <c r="I29">
-        <v>0.4410293066476054</v>
+        <v>0.441</v>
       </c>
       <c r="J29">
-        <v>0.7089552238805971</v>
+        <v>0.709</v>
       </c>
       <c r="K29">
-        <v>0.5224382946896036</v>
+        <v>0.522</v>
       </c>
       <c r="L29">
-        <v>0.5846283074338513</v>
+        <v>0.585</v>
       </c>
       <c r="M29">
-        <v>0.4202954898911353</v>
+        <v>0.42</v>
       </c>
       <c r="N29">
-        <v>0.2043366409408306</v>
+        <v>0.204</v>
       </c>
     </row>
     <row r="30">
@@ -1728,40 +1728,40 @@
         <v>2009</v>
       </c>
       <c r="C30">
-        <v>0.9237526352775826</v>
+        <v>0.924</v>
       </c>
       <c r="D30">
-        <v>0.7638155579021472</v>
+        <v>0.764</v>
       </c>
       <c r="E30">
-        <v>0.7985257985257985</v>
+        <v>0.799</v>
       </c>
       <c r="F30">
-        <v>0.9356868227892345</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="G30">
-        <v>0.7884750527055516</v>
+        <v>0.788</v>
       </c>
       <c r="H30">
-        <v>0.790356394129979</v>
+        <v>0.79</v>
       </c>
       <c r="I30">
-        <v>0.6283712784588441</v>
+        <v>0.628</v>
       </c>
       <c r="J30">
-        <v>0.8008400420021001</v>
+        <v>0.801</v>
       </c>
       <c r="K30">
-        <v>0.712036389083275</v>
+        <v>0.712</v>
       </c>
       <c r="L30">
-        <v>0.5774398868458275</v>
+        <v>0.577</v>
       </c>
       <c r="M30">
-        <v>0.5063069376313946</v>
+        <v>0.506</v>
       </c>
       <c r="N30">
-        <v>0.3192011212333567</v>
+        <v>0.319</v>
       </c>
     </row>
     <row r="31">
@@ -1774,40 +1774,40 @@
         <v>2009</v>
       </c>
       <c r="C31">
-        <v>0.9053888548683405</v>
+        <v>0.905</v>
       </c>
       <c r="D31">
-        <v>0.8541154791154791</v>
+        <v>0.854</v>
       </c>
       <c r="E31">
-        <v>0.8671586715867159</v>
+        <v>0.867</v>
       </c>
       <c r="F31">
-        <v>0.7930717351318209</v>
+        <v>0.793</v>
       </c>
       <c r="G31">
-        <v>0.8802946593001841</v>
+        <v>0.88</v>
       </c>
       <c r="H31">
-        <v>0.761015911872705</v>
+        <v>0.761</v>
       </c>
       <c r="I31">
-        <v>0.6894218942189422</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="J31">
-        <v>0.7867647058823529</v>
+        <v>0.787</v>
       </c>
       <c r="K31">
-        <v>0.6967187979147501</v>
+        <v>0.697</v>
       </c>
       <c r="L31">
-        <v>0.7120515179392825</v>
+        <v>0.712</v>
       </c>
       <c r="M31">
-        <v>0.4192756292203806</v>
+        <v>0.419</v>
       </c>
       <c r="N31">
-        <v>0.3617086662569146</v>
+        <v>0.362</v>
       </c>
     </row>
     <row r="32">
@@ -1820,40 +1820,40 @@
         <v>1999</v>
       </c>
       <c r="C32">
-        <v>0.9319482083709726</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="D32">
-        <v>0.7806552262090484</v>
+        <v>0.781</v>
       </c>
       <c r="E32">
-        <v>0.8133535660091047</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="F32">
-        <v>0.8272394881170019</v>
+        <v>0.827</v>
       </c>
       <c r="G32">
-        <v>0.6806877494626957</v>
+        <v>0.681</v>
       </c>
       <c r="H32">
-        <v>0.7010494752623688</v>
+        <v>0.701</v>
       </c>
       <c r="I32">
-        <v>0.7104945717732207</v>
+        <v>0.71</v>
       </c>
       <c r="J32">
-        <v>0.5869969040247678</v>
+        <v>0.587</v>
       </c>
       <c r="K32">
-        <v>0.6853293413173652</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="L32">
-        <v>0.5882930019620667</v>
+        <v>0.588</v>
       </c>
       <c r="M32">
-        <v>0.2829727843684578</v>
+        <v>0.283</v>
       </c>
       <c r="N32">
-        <v>0.1677215189873418</v>
+        <v>0.168</v>
       </c>
     </row>
     <row r="33">
@@ -1866,40 +1866,40 @@
         <v>2009</v>
       </c>
       <c r="C33">
-        <v>0.8501291989664083</v>
+        <v>0.85</v>
       </c>
       <c r="D33">
-        <v>0.8205033308660251</v>
+        <v>0.821</v>
       </c>
       <c r="E33">
-        <v>0.8635189966801918</v>
+        <v>0.864</v>
       </c>
       <c r="F33">
-        <v>0.8420664206642067</v>
+        <v>0.842</v>
       </c>
       <c r="G33">
-        <v>0.767725258493353</v>
+        <v>0.768</v>
       </c>
       <c r="H33">
-        <v>0.6685103244837758</v>
+        <v>0.669</v>
       </c>
       <c r="I33">
-        <v>0.8048870788596816</v>
+        <v>0.805</v>
       </c>
       <c r="J33">
-        <v>0.7311669128508124</v>
+        <v>0.731</v>
       </c>
       <c r="K33">
-        <v>0.8290251107828656</v>
+        <v>0.829</v>
       </c>
       <c r="L33">
-        <v>0.5011078286558346</v>
+        <v>0.501</v>
       </c>
       <c r="M33">
-        <v>0.2986676535899334</v>
+        <v>0.299</v>
       </c>
       <c r="N33">
-        <v>0.1566888396156689</v>
+        <v>0.157</v>
       </c>
     </row>
     <row r="34">
@@ -1912,40 +1912,40 @@
         <v>2016</v>
       </c>
       <c r="C34">
-        <v>0.8662195552417932</v>
+        <v>0.866</v>
       </c>
       <c r="D34">
-        <v>0.8328621908127208</v>
+        <v>0.833</v>
       </c>
       <c r="E34">
-        <v>0.8691654879773691</v>
+        <v>0.869</v>
       </c>
       <c r="F34">
-        <v>0.7892882311486963</v>
+        <v>0.789</v>
       </c>
       <c r="G34">
-        <v>0.7802896503002472</v>
+        <v>0.78</v>
       </c>
       <c r="H34">
-        <v>0.6699576868829337</v>
+        <v>0.67</v>
       </c>
       <c r="I34">
-        <v>0.7918136908962597</v>
+        <v>0.792</v>
       </c>
       <c r="J34">
-        <v>0.808548216178029</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="K34">
-        <v>0.7992237120677488</v>
+        <v>0.799</v>
       </c>
       <c r="L34">
-        <v>0.5155367231638418</v>
+        <v>0.516</v>
       </c>
       <c r="M34">
-        <v>0.3526912181303116</v>
+        <v>0.353</v>
       </c>
       <c r="N34">
-        <v>0.1425044091710758</v>
+        <v>0.143</v>
       </c>
     </row>
     <row r="35">
@@ -1958,40 +1958,40 @@
         <v>1999</v>
       </c>
       <c r="C35">
-        <v>0.973415877640204</v>
+        <v>0.973</v>
       </c>
       <c r="D35">
-        <v>0.8299733739064283</v>
+        <v>0.83</v>
       </c>
       <c r="E35">
-        <v>0.6103500761035008</v>
+        <v>0.61</v>
       </c>
       <c r="F35">
-        <v>0.9316586627262652</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="G35">
-        <v>0.7419475655430712</v>
+        <v>0.742</v>
       </c>
       <c r="H35">
-        <v>0.5915649278579356</v>
+        <v>0.592</v>
       </c>
       <c r="I35">
-        <v>0.6864188443135811</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="J35">
-        <v>0.593266253869969</v>
+        <v>0.593</v>
       </c>
       <c r="K35">
-        <v>0.6707543664065403</v>
+        <v>0.671</v>
       </c>
       <c r="L35">
-        <v>0.3559935639581657</v>
+        <v>0.356</v>
       </c>
       <c r="M35">
-        <v>0.2367205542725173</v>
+        <v>0.237</v>
       </c>
       <c r="N35">
-        <v>0.1376949410422214</v>
+        <v>0.138</v>
       </c>
     </row>
     <row r="36">
@@ -2004,40 +2004,40 @@
         <v>2009</v>
       </c>
       <c r="C36">
-        <v>0.9143468950749465</v>
+        <v>0.914</v>
       </c>
       <c r="D36">
-        <v>0.7342743172752378</v>
+        <v>0.734</v>
       </c>
       <c r="E36">
-        <v>0.7624885075084278</v>
+        <v>0.762</v>
       </c>
       <c r="F36">
-        <v>0.9195472621596819</v>
+        <v>0.92</v>
       </c>
       <c r="G36">
-        <v>0.7983476132190942</v>
+        <v>0.798</v>
       </c>
       <c r="H36">
-        <v>0.7333333333333333</v>
+        <v>0.733</v>
       </c>
       <c r="I36">
-        <v>0.6299816063764562</v>
+        <v>0.63</v>
       </c>
       <c r="J36">
-        <v>0.6524800979791794</v>
+        <v>0.652</v>
       </c>
       <c r="K36">
-        <v>0.7062423500611995</v>
+        <v>0.706</v>
       </c>
       <c r="L36">
-        <v>0.4236196319018405</v>
+        <v>0.424</v>
       </c>
       <c r="M36">
-        <v>0.2511485451761102</v>
+        <v>0.251</v>
       </c>
       <c r="N36">
-        <v>0.1711573790569504</v>
+        <v>0.171</v>
       </c>
     </row>
     <row r="37">
@@ -2050,40 +2050,40 @@
         <v>2016</v>
       </c>
       <c r="C37">
-        <v>0.9452098686318487</v>
+        <v>0.945</v>
       </c>
       <c r="D37">
-        <v>0.7930038510911425</v>
+        <v>0.793</v>
       </c>
       <c r="E37">
-        <v>0.7878690629011553</v>
+        <v>0.788</v>
       </c>
       <c r="F37">
-        <v>0.9481268011527377</v>
+        <v>0.948</v>
       </c>
       <c r="G37">
-        <v>0.8213256484149856</v>
+        <v>0.821</v>
       </c>
       <c r="H37">
-        <v>0.7733375959079284</v>
+        <v>0.773</v>
       </c>
       <c r="I37">
-        <v>0.7253205128205128</v>
+        <v>0.725</v>
       </c>
       <c r="J37">
-        <v>0.7473549214491825</v>
+        <v>0.747</v>
       </c>
       <c r="K37">
-        <v>0.7963554987212276</v>
+        <v>0.796</v>
       </c>
       <c r="L37">
-        <v>0.4710982658959538</v>
+        <v>0.471</v>
       </c>
       <c r="M37">
-        <v>0.3532991672005125</v>
+        <v>0.353</v>
       </c>
       <c r="N37">
-        <v>0.2423951328850464</v>
+        <v>0.242</v>
       </c>
     </row>
     <row r="38">
@@ -2096,40 +2096,40 @@
         <v>1999</v>
       </c>
       <c r="C38">
-        <v>0.955595026642984</v>
+        <v>0.956</v>
       </c>
       <c r="D38">
-        <v>0.9181216134858519</v>
+        <v>0.918</v>
       </c>
       <c r="E38">
-        <v>0.8995171997585999</v>
+        <v>0.9</v>
       </c>
       <c r="F38">
-        <v>0.8101922490082393</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="G38">
-        <v>0.8879232843871742</v>
+        <v>0.888</v>
       </c>
       <c r="H38">
-        <v>0.9428741445998214</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="I38">
-        <v>0.8808955223880597</v>
+        <v>0.881</v>
       </c>
       <c r="J38">
-        <v>0.821256038647343</v>
+        <v>0.821</v>
       </c>
       <c r="K38">
-        <v>0.7670901391409558</v>
+        <v>0.767</v>
       </c>
       <c r="L38">
-        <v>0.8620581795433219</v>
+        <v>0.862</v>
       </c>
       <c r="M38">
-        <v>0.5933190315660435</v>
+        <v>0.593</v>
       </c>
       <c r="N38">
-        <v>0.4895960832313341</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="39">
@@ -2142,40 +2142,40 @@
         <v>2009</v>
       </c>
       <c r="C39">
-        <v>0.8436991208075545</v>
+        <v>0.844</v>
       </c>
       <c r="D39">
-        <v>0.8476128188358404</v>
+        <v>0.848</v>
       </c>
       <c r="E39">
-        <v>0.8313174239947695</v>
+        <v>0.831</v>
       </c>
       <c r="F39">
-        <v>0.6507988262145419</v>
+        <v>0.651</v>
       </c>
       <c r="G39">
-        <v>0.8686703691604051</v>
+        <v>0.869</v>
       </c>
       <c r="H39">
-        <v>0.7471600129827978</v>
+        <v>0.747</v>
       </c>
       <c r="I39">
-        <v>0.817942819585935</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="J39">
-        <v>0.7176815369586453</v>
+        <v>0.718</v>
       </c>
       <c r="K39">
-        <v>0.6565557729941291</v>
+        <v>0.657</v>
       </c>
       <c r="L39">
-        <v>0.7780678851174935</v>
+        <v>0.778</v>
       </c>
       <c r="M39">
-        <v>0.5677883044756615</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="N39">
-        <v>0.2674494455316373</v>
+        <v>0.267</v>
       </c>
     </row>
     <row r="40">
@@ -2188,40 +2188,40 @@
         <v>2009</v>
       </c>
       <c r="C40">
-        <v>0.9317530606928888</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="D40">
-        <v>0.936358894105373</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="E40">
-        <v>0.9502733663108566</v>
+        <v>0.95</v>
       </c>
       <c r="F40">
-        <v>0.8718016354523872</v>
+        <v>0.872</v>
       </c>
       <c r="G40">
-        <v>0.9664658108462143</v>
+        <v>0.966</v>
       </c>
       <c r="H40">
-        <v>0.9220443985544656</v>
+        <v>0.922</v>
       </c>
       <c r="I40">
-        <v>0.9261408599314165</v>
+        <v>0.926</v>
       </c>
       <c r="J40">
-        <v>0.8995040459410075</v>
+        <v>0.9</v>
       </c>
       <c r="K40">
-        <v>0.7202194357366771</v>
+        <v>0.72</v>
       </c>
       <c r="L40">
-        <v>0.686633533873921</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="M40">
-        <v>0.354635935044526</v>
+        <v>0.355</v>
       </c>
       <c r="N40">
-        <v>0.4289074751698903</v>
+        <v>0.429</v>
       </c>
     </row>
     <row r="41">
@@ -2234,40 +2234,40 @@
         <v>1999</v>
       </c>
       <c r="C41">
-        <v>0.9444682675814752</v>
+        <v>0.944</v>
       </c>
       <c r="D41">
-        <v>0.8014233241505969</v>
+        <v>0.801</v>
       </c>
       <c r="E41">
-        <v>0.8520499108734403</v>
+        <v>0.852</v>
       </c>
       <c r="F41">
-        <v>0.9044821583986075</v>
+        <v>0.904</v>
       </c>
       <c r="G41">
-        <v>0.825184192900201</v>
+        <v>0.825</v>
       </c>
       <c r="H41">
-        <v>0.8400261894369271</v>
+        <v>0.84</v>
       </c>
       <c r="I41">
-        <v>0.6979260595130748</v>
+        <v>0.698</v>
       </c>
       <c r="J41">
-        <v>0.8071687840290381</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="K41">
-        <v>0.7258211678832117</v>
+        <v>0.726</v>
       </c>
       <c r="L41">
-        <v>0.600647099607118</v>
+        <v>0.601</v>
       </c>
       <c r="M41">
-        <v>0.5395818651632606</v>
+        <v>0.54</v>
       </c>
       <c r="N41">
-        <v>0.2771790065604499</v>
+        <v>0.277</v>
       </c>
     </row>
     <row r="42">
@@ -2280,40 +2280,40 @@
         <v>2009</v>
       </c>
       <c r="C42">
-        <v>0.9637784090909091</v>
+        <v>0.964</v>
       </c>
       <c r="D42">
-        <v>0.7845990063875089</v>
+        <v>0.785</v>
       </c>
       <c r="E42">
-        <v>0.8430397727272727</v>
+        <v>0.843</v>
       </c>
       <c r="F42">
-        <v>0.9087681931132411</v>
+        <v>0.909</v>
       </c>
       <c r="G42">
-        <v>0.8839190628328009</v>
+        <v>0.884</v>
       </c>
       <c r="H42">
-        <v>0.8586647727272727</v>
+        <v>0.859</v>
       </c>
       <c r="I42">
-        <v>0.7871357498223169</v>
+        <v>0.787</v>
       </c>
       <c r="J42">
-        <v>0.8931487397941072</v>
+        <v>0.893</v>
       </c>
       <c r="K42">
-        <v>0.8959886403975861</v>
+        <v>0.896</v>
       </c>
       <c r="L42">
-        <v>0.6462851048702453</v>
+        <v>0.646</v>
       </c>
       <c r="M42">
-        <v>0.5688920454545454</v>
+        <v>0.569</v>
       </c>
       <c r="N42">
-        <v>0.2039076376554174</v>
+        <v>0.204</v>
       </c>
     </row>
     <row r="43">
@@ -2326,40 +2326,40 @@
         <v>2016</v>
       </c>
       <c r="C43">
-        <v>0.9303578299345903</v>
+        <v>0.93</v>
       </c>
       <c r="D43">
-        <v>0.7728147862918753</v>
+        <v>0.773</v>
       </c>
       <c r="E43">
-        <v>0.8096339113680154</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F43">
-        <v>0.883011583011583</v>
+        <v>0.883</v>
       </c>
       <c r="G43">
-        <v>0.8521370812475934</v>
+        <v>0.852</v>
       </c>
       <c r="H43">
-        <v>0.8374327440430438</v>
+        <v>0.837</v>
       </c>
       <c r="I43">
-        <v>0.7395151981531358</v>
+        <v>0.74</v>
       </c>
       <c r="J43">
-        <v>0.7960754136206233</v>
+        <v>0.796</v>
       </c>
       <c r="K43">
-        <v>0.8597842835130971</v>
+        <v>0.86</v>
       </c>
       <c r="L43">
-        <v>0.65626204238921</v>
+        <v>0.656</v>
       </c>
       <c r="M43">
-        <v>0.6138117283950617</v>
+        <v>0.614</v>
       </c>
       <c r="N43">
-        <v>0.2603846153846154</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="44">
@@ -2372,40 +2372,40 @@
         <v>2016</v>
       </c>
       <c r="C44">
-        <v>0.9415280665280665</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D44">
-        <v>0.9071949947862357</v>
+        <v>0.907</v>
       </c>
       <c r="E44">
-        <v>0.8660062565172054</v>
+        <v>0.866</v>
       </c>
       <c r="F44">
-        <v>0.9525168655941879</v>
+        <v>0.953</v>
       </c>
       <c r="G44">
-        <v>0.9269750519750519</v>
+        <v>0.927</v>
       </c>
       <c r="H44">
-        <v>0.900103519668737</v>
+        <v>0.9</v>
       </c>
       <c r="I44">
-        <v>0.8976234003656307</v>
+        <v>0.898</v>
       </c>
       <c r="J44">
-        <v>0.8642745709828393</v>
+        <v>0.864</v>
       </c>
       <c r="K44">
-        <v>0.7951244813278008</v>
+        <v>0.795</v>
       </c>
       <c r="L44">
-        <v>0.729497526685759</v>
+        <v>0.729</v>
       </c>
       <c r="M44">
-        <v>0.4784988272087569</v>
+        <v>0.478</v>
       </c>
       <c r="N44">
-        <v>0.3675591369898623</v>
+        <v>0.368</v>
       </c>
     </row>
     <row r="45">
@@ -2418,40 +2418,40 @@
         <v>1999</v>
       </c>
       <c r="C45">
-        <v>0.9762055837563451</v>
+        <v>0.976</v>
       </c>
       <c r="D45">
-        <v>0.8925039872408294</v>
+        <v>0.893</v>
       </c>
       <c r="E45">
-        <v>0.8947704081632653</v>
+        <v>0.895</v>
       </c>
       <c r="F45">
-        <v>0.8953934740882917</v>
+        <v>0.895</v>
       </c>
       <c r="G45">
-        <v>0.7654597885293175</v>
+        <v>0.765</v>
       </c>
       <c r="H45">
-        <v>0.8152967311964455</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="I45">
-        <v>0.8575071724577622</v>
+        <v>0.858</v>
       </c>
       <c r="J45">
-        <v>0.7377102199223803</v>
+        <v>0.738</v>
       </c>
       <c r="K45">
-        <v>0.7832856688910073</v>
+        <v>0.783</v>
       </c>
       <c r="L45">
-        <v>0.6413570274636511</v>
+        <v>0.641</v>
       </c>
       <c r="M45">
-        <v>0.2091754892524864</v>
+        <v>0.209</v>
       </c>
       <c r="N45">
-        <v>0.2851625362085613</v>
+        <v>0.285</v>
       </c>
     </row>
     <row r="46">
@@ -2464,40 +2464,40 @@
         <v>2009</v>
       </c>
       <c r="C46">
-        <v>0.9629554655870445</v>
+        <v>0.963</v>
       </c>
       <c r="D46">
-        <v>0.8574614760746148</v>
+        <v>0.857</v>
       </c>
       <c r="E46">
-        <v>0.9307271622442779</v>
+        <v>0.931</v>
       </c>
       <c r="F46">
-        <v>0.9393081124822982</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="G46">
-        <v>0.9359675785207701</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="H46">
-        <v>0.9709911361804996</v>
+        <v>0.971</v>
       </c>
       <c r="I46">
-        <v>0.9606570675319408</v>
+        <v>0.961</v>
       </c>
       <c r="J46">
-        <v>0.9474964524630043</v>
+        <v>0.947</v>
       </c>
       <c r="K46">
-        <v>0.7430597771023303</v>
+        <v>0.743</v>
       </c>
       <c r="L46">
-        <v>0.8061826316859874</v>
+        <v>0.806</v>
       </c>
       <c r="M46">
-        <v>0.4824294129595775</v>
+        <v>0.482</v>
       </c>
       <c r="N46">
-        <v>0.5514795297932712</v>
+        <v>0.551</v>
       </c>
     </row>
     <row r="47">
@@ -2510,40 +2510,40 @@
         <v>2009</v>
       </c>
       <c r="C47">
-        <v>0.9149066421793695</v>
+        <v>0.915</v>
       </c>
       <c r="D47">
-        <v>0.8344512195121951</v>
+        <v>0.834</v>
       </c>
       <c r="E47">
-        <v>0.8418476598348119</v>
+        <v>0.842</v>
       </c>
       <c r="F47">
-        <v>0.934855403348554</v>
+        <v>0.9350000000000001</v>
       </c>
       <c r="G47">
-        <v>0.8532194079951175</v>
+        <v>0.853</v>
       </c>
       <c r="H47">
-        <v>0.8904026642446261</v>
+        <v>0.89</v>
       </c>
       <c r="I47">
-        <v>0.7358145210494204</v>
+        <v>0.736</v>
       </c>
       <c r="J47">
-        <v>0.7928615009151921</v>
+        <v>0.793</v>
       </c>
       <c r="K47">
-        <v>0.7228475813811986</v>
+        <v>0.723</v>
       </c>
       <c r="L47">
-        <v>0.6479607482367372</v>
+        <v>0.648</v>
       </c>
       <c r="M47">
-        <v>0.5289079229122056</v>
+        <v>0.529</v>
       </c>
       <c r="N47">
-        <v>0.3024954351795496</v>
+        <v>0.302</v>
       </c>
     </row>
     <row r="48">
@@ -2556,40 +2556,40 @@
         <v>1999</v>
       </c>
       <c r="C48">
-        <v>0.9688664183076104</v>
+        <v>0.969</v>
       </c>
       <c r="D48">
-        <v>0.8677455357142857</v>
+        <v>0.868</v>
       </c>
       <c r="E48">
-        <v>0.8288845181230683</v>
+        <v>0.829</v>
       </c>
       <c r="F48">
-        <v>0.8351917323905358</v>
+        <v>0.835</v>
       </c>
       <c r="G48">
-        <v>0.7930848190167477</v>
+        <v>0.793</v>
       </c>
       <c r="H48">
-        <v>0.8370650121391962</v>
+        <v>0.837</v>
       </c>
       <c r="I48">
-        <v>0.6629579375848033</v>
+        <v>0.663</v>
       </c>
       <c r="J48">
-        <v>0.760748185371301</v>
+        <v>0.761</v>
       </c>
       <c r="K48">
-        <v>0.7683057188669161</v>
+        <v>0.768</v>
       </c>
       <c r="L48">
-        <v>0.7580645161290323</v>
+        <v>0.758</v>
       </c>
       <c r="M48">
-        <v>0.4909646927995552</v>
+        <v>0.491</v>
       </c>
       <c r="N48">
-        <v>0.3168678080269436</v>
+        <v>0.317</v>
       </c>
     </row>
     <row r="49">
@@ -2602,40 +2602,40 @@
         <v>2009</v>
       </c>
       <c r="C49">
-        <v>0.9695704057279236</v>
+        <v>0.97</v>
       </c>
       <c r="D49">
-        <v>0.9062312762133014</v>
+        <v>0.906</v>
       </c>
       <c r="E49">
-        <v>0.7790104947526237</v>
+        <v>0.779</v>
       </c>
       <c r="F49">
-        <v>0.8453269632726187</v>
+        <v>0.845</v>
       </c>
       <c r="G49">
-        <v>0.8896860986547085</v>
+        <v>0.89</v>
       </c>
       <c r="H49">
-        <v>0.9063995215311005</v>
+        <v>0.906</v>
       </c>
       <c r="I49">
-        <v>0.9098262432594368</v>
+        <v>0.91</v>
       </c>
       <c r="J49">
-        <v>0.8574843143113235</v>
+        <v>0.857</v>
       </c>
       <c r="K49">
-        <v>0.9097699432327457</v>
+        <v>0.91</v>
       </c>
       <c r="L49">
-        <v>0.7301349325337332</v>
+        <v>0.73</v>
       </c>
       <c r="M49">
-        <v>0.6036494166915943</v>
+        <v>0.604</v>
       </c>
       <c r="N49">
-        <v>0.354066985645933</v>
+        <v>0.354</v>
       </c>
     </row>
     <row r="50">
@@ -2648,40 +2648,40 @@
         <v>2016</v>
       </c>
       <c r="C50">
-        <v>0.9692532942898975</v>
+        <v>0.969</v>
       </c>
       <c r="D50">
-        <v>0.9157863849765259</v>
+        <v>0.916</v>
       </c>
       <c r="E50">
-        <v>0.8371613663133097</v>
+        <v>0.837</v>
       </c>
       <c r="F50">
-        <v>0.8752562225475842</v>
+        <v>0.875</v>
       </c>
       <c r="G50">
-        <v>0.902496328928047</v>
+        <v>0.902</v>
       </c>
       <c r="H50">
-        <v>0.9100467289719626</v>
+        <v>0.91</v>
       </c>
       <c r="I50">
-        <v>0.927629651333138</v>
+        <v>0.928</v>
       </c>
       <c r="J50">
-        <v>0.8278184480234261</v>
+        <v>0.828</v>
       </c>
       <c r="K50">
-        <v>0.9078717201166181</v>
+        <v>0.908</v>
       </c>
       <c r="L50">
-        <v>0.7488276670574443</v>
+        <v>0.749</v>
       </c>
       <c r="M50">
-        <v>0.6400351185250219</v>
+        <v>0.64</v>
       </c>
       <c r="N50">
-        <v>0.416642250219748</v>
+        <v>0.417</v>
       </c>
     </row>
     <row r="51">
@@ -2694,40 +2694,40 @@
         <v>2009</v>
       </c>
       <c r="C51">
-        <v>0.9321872015281757</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="D51">
-        <v>0.8376673040152963</v>
+        <v>0.838</v>
       </c>
       <c r="E51">
-        <v>0.837796480489671</v>
+        <v>0.838</v>
       </c>
       <c r="F51">
-        <v>0.9243697478991597</v>
+        <v>0.924</v>
       </c>
       <c r="G51">
-        <v>0.8792279763042232</v>
+        <v>0.879</v>
       </c>
       <c r="H51">
-        <v>0.9677357770141275</v>
+        <v>0.968</v>
       </c>
       <c r="I51">
-        <v>0.7519572274202788</v>
+        <v>0.752</v>
       </c>
       <c r="J51">
-        <v>0.4255685075482515</v>
+        <v>0.426</v>
       </c>
       <c r="K51">
-        <v>0.9199770817417876</v>
+        <v>0.92</v>
       </c>
       <c r="L51">
-        <v>0.9019870080244555</v>
+        <v>0.902</v>
       </c>
       <c r="M51">
-        <v>0.7585613162425866</v>
+        <v>0.759</v>
       </c>
       <c r="N51">
-        <v>0.6104317921283913</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="52">
@@ -2740,40 +2740,40 @@
         <v>2016</v>
       </c>
       <c r="C52">
-        <v>0.9391708640061992</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="D52">
-        <v>0.8357225881441301</v>
+        <v>0.836</v>
       </c>
       <c r="E52">
-        <v>0.8639007367196588</v>
+        <v>0.864</v>
       </c>
       <c r="F52">
-        <v>0.9236729949631926</v>
+        <v>0.924</v>
       </c>
       <c r="G52">
-        <v>0.8980224893369523</v>
+        <v>0.898</v>
       </c>
       <c r="H52">
-        <v>0.9259976753196435</v>
+        <v>0.926</v>
       </c>
       <c r="I52">
-        <v>0.8206816421378776</v>
+        <v>0.821</v>
       </c>
       <c r="J52">
-        <v>0.4418604651162791</v>
+        <v>0.442</v>
       </c>
       <c r="K52">
-        <v>0.8797983714618069</v>
+        <v>0.88</v>
       </c>
       <c r="L52">
-        <v>0.8503295851105079</v>
+        <v>0.85</v>
       </c>
       <c r="M52">
-        <v>0.6396431342125679</v>
+        <v>0.64</v>
       </c>
       <c r="N52">
-        <v>0.4875968992248062</v>
+        <v>0.488</v>
       </c>
     </row>
     <row r="53">
@@ -2786,40 +2786,40 @@
         <v>2009</v>
       </c>
       <c r="C53">
-        <v>0.8845070422535212</v>
+        <v>0.885</v>
       </c>
       <c r="D53">
-        <v>0.7138810198300283</v>
+        <v>0.714</v>
       </c>
       <c r="E53">
-        <v>0.6807909604519774</v>
+        <v>0.681</v>
       </c>
       <c r="F53">
-        <v>0.6257142857142857</v>
+        <v>0.626</v>
       </c>
       <c r="G53">
-        <v>0.6524216524216524</v>
+        <v>0.652</v>
       </c>
       <c r="H53">
-        <v>0.6901408450704225</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I53">
-        <v>0.7542372881355932</v>
+        <v>0.754</v>
       </c>
       <c r="J53">
-        <v>0.7806267806267806</v>
+        <v>0.781</v>
       </c>
       <c r="K53">
-        <v>0.6440677966101694</v>
+        <v>0.644</v>
       </c>
       <c r="L53">
-        <v>0.4573863636363636</v>
+        <v>0.457</v>
       </c>
       <c r="M53">
-        <v>0.2991452991452991</v>
+        <v>0.299</v>
       </c>
       <c r="N53">
-        <v>0.3286118980169972</v>
+        <v>0.329</v>
       </c>
     </row>
     <row r="54">
@@ -2832,40 +2832,40 @@
         <v>1999</v>
       </c>
       <c r="C54">
-        <v>0.9276785714285715</v>
+        <v>0.928</v>
       </c>
       <c r="D54">
-        <v>0.9030984204131227</v>
+        <v>0.903</v>
       </c>
       <c r="E54">
-        <v>0.8544957472660997</v>
+        <v>0.854</v>
       </c>
       <c r="F54">
-        <v>0.7817901234567901</v>
+        <v>0.782</v>
       </c>
       <c r="G54">
-        <v>0.7951474201474201</v>
+        <v>0.795</v>
       </c>
       <c r="H54">
-        <v>0.8393598103141672</v>
+        <v>0.839</v>
       </c>
       <c r="I54">
-        <v>0.8056473415440072</v>
+        <v>0.806</v>
       </c>
       <c r="J54">
-        <v>0.7598159509202455</v>
+        <v>0.76</v>
       </c>
       <c r="K54">
-        <v>0.7410954803950913</v>
+        <v>0.741</v>
       </c>
       <c r="L54">
-        <v>0.7214611872146118</v>
+        <v>0.721</v>
       </c>
       <c r="M54">
-        <v>0.5653002859866539</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="N54">
-        <v>0.387328543435663</v>
+        <v>0.387</v>
       </c>
     </row>
     <row r="55">
@@ -2878,40 +2878,40 @@
         <v>2009</v>
       </c>
       <c r="C55">
-        <v>0.9004641567818463</v>
+        <v>0.9</v>
       </c>
       <c r="D55">
-        <v>0.7648578811369509</v>
+        <v>0.765</v>
       </c>
       <c r="E55">
-        <v>0.8145077720207254</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="F55">
-        <v>0.7449664429530202</v>
+        <v>0.745</v>
       </c>
       <c r="G55">
-        <v>0.7713769051924567</v>
+        <v>0.771</v>
       </c>
       <c r="H55">
-        <v>0.8060355945318545</v>
+        <v>0.806</v>
       </c>
       <c r="I55">
-        <v>0.8908432488360062</v>
+        <v>0.891</v>
       </c>
       <c r="J55">
-        <v>0.8222222222222222</v>
+        <v>0.822</v>
       </c>
       <c r="K55">
-        <v>0.7652061855670103</v>
+        <v>0.765</v>
       </c>
       <c r="L55">
-        <v>0.7009055627425614</v>
+        <v>0.701</v>
       </c>
       <c r="M55">
-        <v>0.4276111685625646</v>
+        <v>0.428</v>
       </c>
       <c r="N55">
-        <v>0.2751227073107724</v>
+        <v>0.275</v>
       </c>
     </row>
     <row r="56">
@@ -2924,40 +2924,40 @@
         <v>2016</v>
       </c>
       <c r="C56">
-        <v>0.9314301707248811</v>
+        <v>0.931</v>
       </c>
       <c r="D56">
-        <v>0.7544792833146696</v>
+        <v>0.754</v>
       </c>
       <c r="E56">
-        <v>0.800390843104411</v>
+        <v>0.8</v>
       </c>
       <c r="F56">
-        <v>0.7642458100558659</v>
+        <v>0.764</v>
       </c>
       <c r="G56">
-        <v>0.8087783058428851</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="H56">
-        <v>0.7889321468298109</v>
+        <v>0.789</v>
       </c>
       <c r="I56">
-        <v>0.8851540616246498</v>
+        <v>0.885</v>
       </c>
       <c r="J56">
-        <v>0.9075677185143814</v>
+        <v>0.908</v>
       </c>
       <c r="K56">
-        <v>0.7509065550906555</v>
+        <v>0.751</v>
       </c>
       <c r="L56">
-        <v>0.6631225517627308</v>
+        <v>0.663</v>
       </c>
       <c r="M56">
-        <v>0.467972027972028</v>
+        <v>0.468</v>
       </c>
       <c r="N56">
-        <v>0.2977715877437326</v>
+        <v>0.298</v>
       </c>
     </row>
     <row r="57">
@@ -2970,40 +2970,40 @@
         <v>2009</v>
       </c>
       <c r="C57">
-        <v>0.8821555881736213</v>
+        <v>0.882</v>
       </c>
       <c r="D57">
-        <v>0.7499472907442547</v>
+        <v>0.75</v>
       </c>
       <c r="E57">
-        <v>0.6653302384469297</v>
+        <v>0.665</v>
       </c>
       <c r="F57">
-        <v>0.6792095858734497</v>
+        <v>0.679</v>
       </c>
       <c r="G57">
-        <v>0.7476300821571519</v>
+        <v>0.748</v>
       </c>
       <c r="H57">
-        <v>0.7716617831728757</v>
+        <v>0.772</v>
       </c>
       <c r="I57">
-        <v>0.726488533557753</v>
+        <v>0.726</v>
       </c>
       <c r="J57">
-        <v>0.8067297581493165</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="K57">
-        <v>0.6701592623637888</v>
+        <v>0.67</v>
       </c>
       <c r="L57">
-        <v>0.6146557169930512</v>
+        <v>0.615</v>
       </c>
       <c r="M57">
-        <v>0.3764977927265083</v>
+        <v>0.376</v>
       </c>
       <c r="N57">
-        <v>0.3105407111298127</v>
+        <v>0.311</v>
       </c>
     </row>
     <row r="58">
@@ -3016,40 +3016,40 @@
         <v>1999</v>
       </c>
       <c r="C58">
-        <v>0.9088699878493317</v>
+        <v>0.909</v>
       </c>
       <c r="D58">
-        <v>0.7932773109243697</v>
+        <v>0.793</v>
       </c>
       <c r="E58">
-        <v>0.7258064516129032</v>
+        <v>0.726</v>
       </c>
       <c r="F58">
-        <v>0.8013923013923014</v>
+        <v>0.801</v>
       </c>
       <c r="G58">
-        <v>0.7608785743887277</v>
+        <v>0.761</v>
       </c>
       <c r="H58">
-        <v>0.7649918962722853</v>
+        <v>0.765</v>
       </c>
       <c r="I58">
-        <v>0.7223587223587223</v>
+        <v>0.722</v>
       </c>
       <c r="J58">
-        <v>0.6655546288573811</v>
+        <v>0.666</v>
       </c>
       <c r="K58">
-        <v>0.6704684317718941</v>
+        <v>0.67</v>
       </c>
       <c r="L58">
-        <v>0.6434108527131783</v>
+        <v>0.643</v>
       </c>
       <c r="M58">
-        <v>0.4361839278040395</v>
+        <v>0.436</v>
       </c>
       <c r="N58">
-        <v>0.3020425901781834</v>
+        <v>0.302</v>
       </c>
     </row>
     <row r="59">
@@ -3062,40 +3062,40 @@
         <v>2009</v>
       </c>
       <c r="C59">
-        <v>0.8116048475945649</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="D59">
-        <v>0.8422214049282825</v>
+        <v>0.842</v>
       </c>
       <c r="E59">
-        <v>0.7986008836524301</v>
+        <v>0.799</v>
       </c>
       <c r="F59">
-        <v>0.721588819418904</v>
+        <v>0.722</v>
       </c>
       <c r="G59">
-        <v>0.7937384898710865</v>
+        <v>0.794</v>
       </c>
       <c r="H59">
-        <v>0.8252106998900697</v>
+        <v>0.825</v>
       </c>
       <c r="I59">
-        <v>0.7012509197939661</v>
+        <v>0.701</v>
       </c>
       <c r="J59">
-        <v>0.6595588235294118</v>
+        <v>0.66</v>
       </c>
       <c r="K59">
-        <v>0.8202494497432135</v>
+        <v>0.82</v>
       </c>
       <c r="L59">
-        <v>0.6589147286821705</v>
+        <v>0.659</v>
       </c>
       <c r="M59">
-        <v>0.5486953325983095</v>
+        <v>0.549</v>
       </c>
       <c r="N59">
-        <v>0.3718703976435935</v>
+        <v>0.372</v>
       </c>
     </row>
     <row r="60">
@@ -3108,40 +3108,40 @@
         <v>2016</v>
       </c>
       <c r="C60">
-        <v>0.8837726262305494</v>
+        <v>0.884</v>
       </c>
       <c r="D60">
-        <v>0.8236975857687421</v>
+        <v>0.824</v>
       </c>
       <c r="E60">
-        <v>0.7839821314613912</v>
+        <v>0.784</v>
       </c>
       <c r="F60">
-        <v>0.7328050713153724</v>
+        <v>0.733</v>
       </c>
       <c r="G60">
-        <v>0.8401652367333969</v>
+        <v>0.84</v>
       </c>
       <c r="H60">
-        <v>0.7910872313527181</v>
+        <v>0.791</v>
       </c>
       <c r="I60">
-        <v>0.8046924540266328</v>
+        <v>0.805</v>
       </c>
       <c r="J60">
-        <v>0.8168835290384006</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="K60">
-        <v>0.7845373891001267</v>
+        <v>0.785</v>
       </c>
       <c r="L60">
-        <v>0.5207933461292387</v>
+        <v>0.521</v>
       </c>
       <c r="M60">
-        <v>0.4704198473282443</v>
+        <v>0.47</v>
       </c>
       <c r="N60">
-        <v>0.329946014607812</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="61">
@@ -3154,40 +3154,40 @@
         <v>2009</v>
       </c>
       <c r="C61">
-        <v>0.8710833982852689</v>
+        <v>0.871</v>
       </c>
       <c r="D61">
-        <v>0.8632276384287743</v>
+        <v>0.863</v>
       </c>
       <c r="E61">
-        <v>0.8407512626262627</v>
+        <v>0.841</v>
       </c>
       <c r="F61">
-        <v>0.8796641791044776</v>
+        <v>0.88</v>
       </c>
       <c r="G61">
-        <v>0.9030837004405287</v>
+        <v>0.903</v>
       </c>
       <c r="H61">
-        <v>0.869856608478803</v>
+        <v>0.87</v>
       </c>
       <c r="I61">
-        <v>0.8161413562559694</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="J61">
-        <v>0.7844000629029722</v>
+        <v>0.784</v>
       </c>
       <c r="K61">
-        <v>0.7379234629861983</v>
+        <v>0.738</v>
       </c>
       <c r="L61">
-        <v>0.6685588142541785</v>
+        <v>0.669</v>
       </c>
       <c r="M61">
-        <v>0.5155632801390425</v>
+        <v>0.516</v>
       </c>
       <c r="N61">
-        <v>0.4135220125786164</v>
+        <v>0.414</v>
       </c>
     </row>
     <row r="62">
@@ -3200,40 +3200,40 @@
         <v>2016</v>
       </c>
       <c r="C62">
-        <v>0.8753981637624133</v>
+        <v>0.875</v>
       </c>
       <c r="D62">
-        <v>0.885233644859813</v>
+        <v>0.885</v>
       </c>
       <c r="E62">
-        <v>0.8744151225903051</v>
+        <v>0.874</v>
       </c>
       <c r="F62">
-        <v>0.8596886137685237</v>
+        <v>0.86</v>
       </c>
       <c r="G62">
-        <v>0.9166510582506088</v>
+        <v>0.917</v>
       </c>
       <c r="H62">
-        <v>0.8487940630797773</v>
+        <v>0.849</v>
       </c>
       <c r="I62">
-        <v>0.8362231436110064</v>
+        <v>0.836</v>
       </c>
       <c r="J62">
-        <v>0.7963240810202551</v>
+        <v>0.796</v>
       </c>
       <c r="K62">
-        <v>0.778255184008967</v>
+        <v>0.778</v>
       </c>
       <c r="L62">
-        <v>0.7045497097921738</v>
+        <v>0.705</v>
       </c>
       <c r="M62">
-        <v>0.5881690140845071</v>
+        <v>0.588</v>
       </c>
       <c r="N62">
-        <v>0.4674501025927998</v>
+        <v>0.467</v>
       </c>
     </row>
     <row r="63">
@@ -3246,40 +3246,40 @@
         <v>2009</v>
       </c>
       <c r="C63">
-        <v>0.917221693625119</v>
+        <v>0.917</v>
       </c>
       <c r="D63">
-        <v>0.8250478011472275</v>
+        <v>0.825</v>
       </c>
       <c r="E63">
-        <v>0.7951172809956917</v>
+        <v>0.795</v>
       </c>
       <c r="F63">
-        <v>0.8608986615678776</v>
+        <v>0.861</v>
       </c>
       <c r="G63">
-        <v>0.8273553323768532</v>
+        <v>0.827</v>
       </c>
       <c r="H63">
-        <v>0.8312796208530806</v>
+        <v>0.831</v>
       </c>
       <c r="I63">
-        <v>0.738255033557047</v>
+        <v>0.738</v>
       </c>
       <c r="J63">
-        <v>0.8277010947168015</v>
+        <v>0.828</v>
       </c>
       <c r="K63">
-        <v>0.6641184902054468</v>
+        <v>0.664</v>
       </c>
       <c r="L63">
-        <v>0.6208712302537099</v>
+        <v>0.621</v>
       </c>
       <c r="M63">
-        <v>0.3741007194244604</v>
+        <v>0.374</v>
       </c>
       <c r="N63">
-        <v>0.3579952267303103</v>
+        <v>0.358</v>
       </c>
     </row>
     <row r="64">
@@ -3292,40 +3292,40 @@
         <v>2016</v>
       </c>
       <c r="C64">
-        <v>0.9234806629834255</v>
+        <v>0.923</v>
       </c>
       <c r="D64">
-        <v>0.848686030428769</v>
+        <v>0.849</v>
       </c>
       <c r="E64">
-        <v>0.8026024363233666</v>
+        <v>0.803</v>
       </c>
       <c r="F64">
-        <v>0.8342556723851687</v>
+        <v>0.834</v>
       </c>
       <c r="G64">
-        <v>0.8338870431893688</v>
+        <v>0.834</v>
       </c>
       <c r="H64">
-        <v>0.7894159583219085</v>
+        <v>0.789</v>
       </c>
       <c r="I64">
-        <v>0.7243963363863447</v>
+        <v>0.724</v>
       </c>
       <c r="J64">
-        <v>0.837055417700579</v>
+        <v>0.837</v>
       </c>
       <c r="K64">
-        <v>0.6873278236914601</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="L64">
-        <v>0.6326135105204873</v>
+        <v>0.633</v>
       </c>
       <c r="M64">
-        <v>0.4276187829952764</v>
+        <v>0.428</v>
       </c>
       <c r="N64">
-        <v>0.330300523848911</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="65">
@@ -3338,40 +3338,40 @@
         <v>2009</v>
       </c>
       <c r="C65">
-        <v>0.7315010570824524</v>
+        <v>0.732</v>
       </c>
       <c r="D65">
-        <v>0.7231907025884838</v>
+        <v>0.723</v>
       </c>
       <c r="E65">
-        <v>0.7053524112347642</v>
+        <v>0.705</v>
       </c>
       <c r="F65">
-        <v>0.7761351636747624</v>
+        <v>0.776</v>
       </c>
       <c r="G65">
-        <v>0.7186673717609731</v>
+        <v>0.719</v>
       </c>
       <c r="H65">
-        <v>0.7547368421052632</v>
+        <v>0.755</v>
       </c>
       <c r="I65">
-        <v>0.4604847207586933</v>
+        <v>0.46</v>
       </c>
       <c r="J65">
-        <v>0.804865150713908</v>
+        <v>0.805</v>
       </c>
       <c r="K65">
-        <v>0.6684238270954138</v>
+        <v>0.668</v>
       </c>
       <c r="L65">
-        <v>0.3824933687002652</v>
+        <v>0.382</v>
       </c>
       <c r="M65">
-        <v>0.3909138932910723</v>
+        <v>0.391</v>
       </c>
       <c r="N65">
-        <v>0.3178947368421053</v>
+        <v>0.318</v>
       </c>
     </row>
     <row r="66">
@@ -3384,40 +3384,40 @@
         <v>2016</v>
       </c>
       <c r="C66">
-        <v>0.8548153511947864</v>
+        <v>0.855</v>
       </c>
       <c r="D66">
-        <v>0.720492396813903</v>
+        <v>0.72</v>
       </c>
       <c r="E66">
-        <v>0.7119505993461678</v>
+        <v>0.712</v>
       </c>
       <c r="F66">
-        <v>0.8529518290474466</v>
+        <v>0.853</v>
       </c>
       <c r="G66">
-        <v>0.7043478260869566</v>
+        <v>0.704</v>
       </c>
       <c r="H66">
-        <v>0.7356446370530878</v>
+        <v>0.736</v>
       </c>
       <c r="I66">
-        <v>0.5394641564083997</v>
+        <v>0.539</v>
       </c>
       <c r="J66">
-        <v>0.8547687861271677</v>
+        <v>0.855</v>
       </c>
       <c r="K66">
-        <v>0.7061799783158655</v>
+        <v>0.706</v>
       </c>
       <c r="L66">
-        <v>0.3560551124002901</v>
+        <v>0.356</v>
       </c>
       <c r="M66">
-        <v>0.4002169197396963</v>
+        <v>0.4</v>
       </c>
       <c r="N66">
-        <v>0.2811143270622287</v>
+        <v>0.281</v>
       </c>
     </row>
     <row r="67">
@@ -3430,40 +3430,40 @@
         <v>1999</v>
       </c>
       <c r="C67">
-        <v>0.9477124183006536</v>
+        <v>0.948</v>
       </c>
       <c r="D67">
-        <v>0.9029280712921706</v>
+        <v>0.903</v>
       </c>
       <c r="E67">
-        <v>0.827120822622108</v>
+        <v>0.827</v>
       </c>
       <c r="F67">
-        <v>0.7797524595366551</v>
+        <v>0.78</v>
       </c>
       <c r="G67">
-        <v>0.9056603773584906</v>
+        <v>0.906</v>
       </c>
       <c r="H67">
-        <v>0.7137059007180768</v>
+        <v>0.714</v>
       </c>
       <c r="I67">
-        <v>0.497148288973384</v>
+        <v>0.497</v>
       </c>
       <c r="J67">
-        <v>0.6473802635808422</v>
+        <v>0.647</v>
       </c>
       <c r="K67">
-        <v>0.6705220381369178</v>
+        <v>0.671</v>
       </c>
       <c r="L67">
-        <v>0.6759410801963993</v>
+        <v>0.676</v>
       </c>
       <c r="M67">
-        <v>0.3618925831202046</v>
+        <v>0.362</v>
       </c>
       <c r="N67">
-        <v>0.2097235462345091</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="68">
@@ -3476,40 +3476,40 @@
         <v>2009</v>
       </c>
       <c r="C68">
-        <v>0.8836071303739951</v>
+        <v>0.884</v>
       </c>
       <c r="D68">
-        <v>0.8673647469458988</v>
+        <v>0.867</v>
       </c>
       <c r="E68">
-        <v>0.8749563395040167</v>
+        <v>0.875</v>
       </c>
       <c r="F68">
-        <v>0.8561452513966481</v>
+        <v>0.856</v>
       </c>
       <c r="G68">
-        <v>0.8966237382526975</v>
+        <v>0.897</v>
       </c>
       <c r="H68">
-        <v>0.8795013850415513</v>
+        <v>0.88</v>
       </c>
       <c r="I68">
-        <v>0.7300313916986397</v>
+        <v>0.73</v>
       </c>
       <c r="J68">
-        <v>0.8598814918089926</v>
+        <v>0.86</v>
       </c>
       <c r="K68">
-        <v>0.8009708737864077</v>
+        <v>0.801</v>
       </c>
       <c r="L68">
-        <v>0.6973821989528796</v>
+        <v>0.697</v>
       </c>
       <c r="M68">
-        <v>0.5019210618232623</v>
+        <v>0.502</v>
       </c>
       <c r="N68">
-        <v>0.4025748086290884</v>
+        <v>0.403</v>
       </c>
     </row>
     <row r="69">
@@ -3522,40 +3522,40 @@
         <v>2016</v>
       </c>
       <c r="C69">
-        <v>0.9283478833800033</v>
+        <v>0.928</v>
       </c>
       <c r="D69">
-        <v>0.8106411103767349</v>
+        <v>0.8110000000000001</v>
       </c>
       <c r="E69">
-        <v>0.8550628722700199</v>
+        <v>0.855</v>
       </c>
       <c r="F69">
-        <v>0.8520231213872832</v>
+        <v>0.852</v>
       </c>
       <c r="G69">
-        <v>0.8560105680317041</v>
+        <v>0.856</v>
       </c>
       <c r="H69">
-        <v>0.8694225721784777</v>
+        <v>0.869</v>
       </c>
       <c r="I69">
-        <v>0.7471511147811726</v>
+        <v>0.747</v>
       </c>
       <c r="J69">
-        <v>0.8714144411473789</v>
+        <v>0.871</v>
       </c>
       <c r="K69">
-        <v>0.7368940016433854</v>
+        <v>0.737</v>
       </c>
       <c r="L69">
-        <v>0.6092297476759628</v>
+        <v>0.609</v>
       </c>
       <c r="M69">
-        <v>0.4791941875825628</v>
+        <v>0.479</v>
       </c>
       <c r="N69">
-        <v>0.2943309162821358</v>
+        <v>0.294</v>
       </c>
     </row>
     <row r="70">
@@ -3568,40 +3568,40 @@
         <v>2009</v>
       </c>
       <c r="C70">
-        <v>0.8979010106245141</v>
+        <v>0.898</v>
       </c>
       <c r="D70">
-        <v>0.7352787910369984</v>
+        <v>0.735</v>
       </c>
       <c r="E70">
-        <v>0.7816331854943909</v>
+        <v>0.782</v>
       </c>
       <c r="F70">
-        <v>0.9237947122861586</v>
+        <v>0.924</v>
       </c>
       <c r="G70">
-        <v>0.7808433107756377</v>
+        <v>0.781</v>
       </c>
       <c r="H70">
-        <v>0.8358324715615305</v>
+        <v>0.836</v>
       </c>
       <c r="I70">
-        <v>0.7019505851755526</v>
+        <v>0.702</v>
       </c>
       <c r="J70">
-        <v>0.7878473123863932</v>
+        <v>0.788</v>
       </c>
       <c r="K70">
-        <v>0.6916883116883117</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="L70">
-        <v>0.5292580982236155</v>
+        <v>0.529</v>
       </c>
       <c r="M70">
-        <v>0.4427640156453716</v>
+        <v>0.443</v>
       </c>
       <c r="N70">
-        <v>0.2609261186264308</v>
+        <v>0.261</v>
       </c>
     </row>
     <row r="71">
@@ -3614,40 +3614,40 @@
         <v>2016</v>
       </c>
       <c r="C71">
-        <v>0.9235541324794877</v>
+        <v>0.924</v>
       </c>
       <c r="D71">
-        <v>0.9250099720781811</v>
+        <v>0.925</v>
       </c>
       <c r="E71">
-        <v>0.8835493519441675</v>
+        <v>0.884</v>
       </c>
       <c r="F71">
-        <v>0.8211788211788211</v>
+        <v>0.821</v>
       </c>
       <c r="G71">
-        <v>0.9490814696485623</v>
+        <v>0.949</v>
       </c>
       <c r="H71">
-        <v>0.9512724403235352</v>
+        <v>0.951</v>
       </c>
       <c r="I71">
-        <v>0.9401197604790419</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J71">
-        <v>0.9197138314785374</v>
+        <v>0.92</v>
       </c>
       <c r="K71">
-        <v>0.7755467196819086</v>
+        <v>0.776</v>
       </c>
       <c r="L71">
-        <v>0.7080087876972239</v>
+        <v>0.708</v>
       </c>
       <c r="M71">
-        <v>0.4772545889864326</v>
+        <v>0.477</v>
       </c>
       <c r="N71">
-        <v>0.558291956305859</v>
+        <v>0.5580000000000001</v>
       </c>
     </row>
     <row r="72">
@@ -3660,40 +3660,40 @@
         <v>1999</v>
       </c>
       <c r="C72">
-        <v>0.9608669476219145</v>
+        <v>0.961</v>
       </c>
       <c r="D72">
-        <v>0.8171942892613284</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="E72">
-        <v>0.906934306569343</v>
+        <v>0.907</v>
       </c>
       <c r="F72">
-        <v>0.749535027898326</v>
+        <v>0.75</v>
       </c>
       <c r="G72">
-        <v>0.7827818627450981</v>
+        <v>0.783</v>
       </c>
       <c r="H72">
-        <v>0.9138452237001209</v>
+        <v>0.914</v>
       </c>
       <c r="I72">
-        <v>0.898418491484185</v>
+        <v>0.898</v>
       </c>
       <c r="J72">
-        <v>0.8164400494437577</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="K72">
-        <v>0.8605710814094775</v>
+        <v>0.861</v>
       </c>
       <c r="L72">
-        <v>0.7660550458715596</v>
+        <v>0.766</v>
       </c>
       <c r="M72">
-        <v>0.5531848133040477</v>
+        <v>0.553</v>
       </c>
       <c r="N72">
-        <v>0.3867298578199052</v>
+        <v>0.387</v>
       </c>
     </row>
     <row r="73">
@@ -3706,40 +3706,40 @@
         <v>2009</v>
       </c>
       <c r="C73">
-        <v>0.8504788384306456</v>
+        <v>0.85</v>
       </c>
       <c r="D73">
-        <v>0.8506211180124224</v>
+        <v>0.851</v>
       </c>
       <c r="E73">
-        <v>0.7593798449612403</v>
+        <v>0.759</v>
       </c>
       <c r="F73">
-        <v>0.6411764705882353</v>
+        <v>0.641</v>
       </c>
       <c r="G73">
-        <v>0.8170844939647168</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="H73">
-        <v>0.8906732550957381</v>
+        <v>0.891</v>
       </c>
       <c r="I73">
-        <v>0.9129894344313239</v>
+        <v>0.913</v>
       </c>
       <c r="J73">
-        <v>0.7638502011761065</v>
+        <v>0.764</v>
       </c>
       <c r="K73">
-        <v>0.794998456313677</v>
+        <v>0.795</v>
       </c>
       <c r="L73">
-        <v>0.6870937790157846</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="M73">
-        <v>0.4342715743891123</v>
+        <v>0.434</v>
       </c>
       <c r="N73">
-        <v>0.2694925742574257</v>
+        <v>0.269</v>
       </c>
     </row>
     <row r="74">
@@ -3752,40 +3752,40 @@
         <v>1999</v>
       </c>
       <c r="C74">
-        <v>0.9698018244731047</v>
+        <v>0.97</v>
       </c>
       <c r="D74">
-        <v>0.8832620848405129</v>
+        <v>0.883</v>
       </c>
       <c r="E74">
-        <v>0.939595192915876</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F74">
-        <v>0.8163001293661061</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G74">
-        <v>0.9213447510307643</v>
+        <v>0.921</v>
       </c>
       <c r="H74">
-        <v>0.7138728323699421</v>
+        <v>0.714</v>
       </c>
       <c r="I74">
-        <v>0.7227025296189561</v>
+        <v>0.723</v>
       </c>
       <c r="J74">
-        <v>0.8279084756687077</v>
+        <v>0.828</v>
       </c>
       <c r="K74">
-        <v>0.8154330708661417</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="L74">
-        <v>0.7336037863421231</v>
+        <v>0.734</v>
       </c>
       <c r="M74">
-        <v>0.398562561254492</v>
+        <v>0.399</v>
       </c>
       <c r="N74">
-        <v>0.3622246298302637</v>
+        <v>0.362</v>
       </c>
     </row>
     <row r="75">
@@ -3798,40 +3798,40 @@
         <v>2009</v>
       </c>
       <c r="C75">
-        <v>0.9099186991869919</v>
+        <v>0.91</v>
       </c>
       <c r="D75">
-        <v>0.914034516444155</v>
+        <v>0.914</v>
       </c>
       <c r="E75">
-        <v>0.8426047120418848</v>
+        <v>0.843</v>
       </c>
       <c r="F75">
-        <v>0.8778576094056172</v>
+        <v>0.878</v>
       </c>
       <c r="G75">
-        <v>0.9595959595959596</v>
+        <v>0.96</v>
       </c>
       <c r="H75">
-        <v>0.7626359564939219</v>
+        <v>0.763</v>
       </c>
       <c r="I75">
-        <v>0.9360877985797289</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="J75">
-        <v>0.8495145631067961</v>
+        <v>0.85</v>
       </c>
       <c r="K75">
-        <v>0.6118484946584655</v>
+        <v>0.612</v>
       </c>
       <c r="L75">
-        <v>0.6528952504879636</v>
+        <v>0.653</v>
       </c>
       <c r="M75">
-        <v>0.2667103538663172</v>
+        <v>0.267</v>
       </c>
       <c r="N75">
-        <v>0.5268087855297158</v>
+        <v>0.527</v>
       </c>
     </row>
     <row r="76">
@@ -3844,40 +3844,40 @@
         <v>1999</v>
       </c>
       <c r="C76">
-        <v>0.9359283499827764</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="D76">
-        <v>0.8858965272856131</v>
+        <v>0.886</v>
       </c>
       <c r="E76">
-        <v>0.9009584664536742</v>
+        <v>0.901</v>
       </c>
       <c r="F76">
-        <v>0.8077794561933535</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="G76">
-        <v>0.8786919831223629</v>
+        <v>0.879</v>
       </c>
       <c r="H76">
-        <v>0.9205298013245033</v>
+        <v>0.921</v>
       </c>
       <c r="I76">
-        <v>0.8747361013370866</v>
+        <v>0.875</v>
       </c>
       <c r="J76">
-        <v>0.8478731074260994</v>
+        <v>0.848</v>
       </c>
       <c r="K76">
-        <v>0.7816608996539792</v>
+        <v>0.782</v>
       </c>
       <c r="L76">
-        <v>0.6804780876494024</v>
+        <v>0.68</v>
       </c>
       <c r="M76">
-        <v>0.5632745024408562</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="N76">
-        <v>0.5421779141104295</v>
+        <v>0.542</v>
       </c>
     </row>
     <row r="77">
@@ -3890,40 +3890,40 @@
         <v>1999</v>
       </c>
       <c r="C77">
-        <v>0.9354684512428298</v>
+        <v>0.9350000000000001</v>
       </c>
       <c r="D77">
-        <v>0.7842465753424658</v>
+        <v>0.784</v>
       </c>
       <c r="E77">
-        <v>0.8254580520732884</v>
+        <v>0.825</v>
       </c>
       <c r="F77">
-        <v>0.8865929841422393</v>
+        <v>0.887</v>
       </c>
       <c r="G77">
-        <v>0.8015303682448589</v>
+        <v>0.802</v>
       </c>
       <c r="H77">
-        <v>0.7910518800571157</v>
+        <v>0.791</v>
       </c>
       <c r="I77">
-        <v>0.7476007677543186</v>
+        <v>0.748</v>
       </c>
       <c r="J77">
-        <v>0.5004940711462451</v>
+        <v>0.5</v>
       </c>
       <c r="K77">
-        <v>0.7252273815222594</v>
+        <v>0.725</v>
       </c>
       <c r="L77">
-        <v>0.8368446839784419</v>
+        <v>0.837</v>
       </c>
       <c r="M77">
-        <v>0.2684290798169802</v>
+        <v>0.268</v>
       </c>
       <c r="N77">
-        <v>0.2048314041268244</v>
+        <v>0.205</v>
       </c>
     </row>
     <row r="78">
@@ -3936,40 +3936,40 @@
         <v>2009</v>
       </c>
       <c r="C78">
-        <v>0.8663063909774437</v>
+        <v>0.866</v>
       </c>
       <c r="D78">
-        <v>0.8267012008476572</v>
+        <v>0.827</v>
       </c>
       <c r="E78">
-        <v>0.8011310084825636</v>
+        <v>0.801</v>
       </c>
       <c r="F78">
-        <v>0.8209586466165414</v>
+        <v>0.821</v>
       </c>
       <c r="G78">
-        <v>0.8772384542884072</v>
+        <v>0.877</v>
       </c>
       <c r="H78">
-        <v>0.8305640065527732</v>
+        <v>0.831</v>
       </c>
       <c r="I78">
-        <v>0.8945489169245417</v>
+        <v>0.895</v>
       </c>
       <c r="J78">
-        <v>0.8487058823529412</v>
+        <v>0.849</v>
       </c>
       <c r="K78">
-        <v>0.8049411764705883</v>
+        <v>0.805</v>
       </c>
       <c r="L78">
-        <v>0.6799340555817239</v>
+        <v>0.68</v>
       </c>
       <c r="M78">
-        <v>0.4535790219702339</v>
+        <v>0.454</v>
       </c>
       <c r="N78">
-        <v>0.449329884787209</v>
+        <v>0.449</v>
       </c>
     </row>
     <row r="79">
@@ -3982,40 +3982,40 @@
         <v>2016</v>
       </c>
       <c r="C79">
-        <v>0.907082700538451</v>
+        <v>0.907</v>
       </c>
       <c r="D79">
-        <v>0.808154803040774</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="E79">
-        <v>0.8144159072079536</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="F79">
-        <v>0.8363686534216336</v>
+        <v>0.836</v>
       </c>
       <c r="G79">
-        <v>0.8868159203980099</v>
+        <v>0.887</v>
       </c>
       <c r="H79">
-        <v>0.7604295745559686</v>
+        <v>0.76</v>
       </c>
       <c r="I79">
-        <v>0.9319972356599862</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="J79">
-        <v>0.881695196024296</v>
+        <v>0.882</v>
       </c>
       <c r="K79">
-        <v>0.8068338385230091</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="L79">
-        <v>0.6356353591160221</v>
+        <v>0.636</v>
       </c>
       <c r="M79">
-        <v>0.4916262975778547</v>
+        <v>0.492</v>
       </c>
       <c r="N79">
-        <v>0.4973778636489097</v>
+        <v>0.497</v>
       </c>
     </row>
     <row r="80">
@@ -4028,40 +4028,40 @@
         <v>1999</v>
       </c>
       <c r="C80">
-        <v>0.9848573092603378</v>
+        <v>0.985</v>
       </c>
       <c r="D80">
-        <v>0.9313089622641509</v>
+        <v>0.931</v>
       </c>
       <c r="E80">
-        <v>0.872106824925816</v>
+        <v>0.872</v>
       </c>
       <c r="F80">
-        <v>0.9680726420620972</v>
+        <v>0.968</v>
       </c>
       <c r="G80">
-        <v>0.8593978368897983</v>
+        <v>0.859</v>
       </c>
       <c r="H80">
-        <v>0.9074992704989787</v>
+        <v>0.907</v>
       </c>
       <c r="I80">
-        <v>0.7254038179148311</v>
+        <v>0.725</v>
       </c>
       <c r="J80">
-        <v>0.6987698769876988</v>
+        <v>0.699</v>
       </c>
       <c r="K80">
-        <v>0.7960680751173709</v>
+        <v>0.796</v>
       </c>
       <c r="L80">
-        <v>0.722645534897897</v>
+        <v>0.723</v>
       </c>
       <c r="M80">
-        <v>0.4955726092089728</v>
+        <v>0.496</v>
       </c>
       <c r="N80">
-        <v>0.2097310365669386</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="81">
@@ -4074,40 +4074,40 @@
         <v>2009</v>
       </c>
       <c r="C81">
-        <v>0.9114565731666103</v>
+        <v>0.911</v>
       </c>
       <c r="D81">
-        <v>0.8438030560271647</v>
+        <v>0.844</v>
       </c>
       <c r="E81">
-        <v>0.7548321464903357</v>
+        <v>0.755</v>
       </c>
       <c r="F81">
-        <v>0.6990521327014217</v>
+        <v>0.699</v>
       </c>
       <c r="G81">
-        <v>0.844354018311292</v>
+        <v>0.844</v>
       </c>
       <c r="H81">
-        <v>0.7813450490030416</v>
+        <v>0.781</v>
       </c>
       <c r="I81">
-        <v>0.6682528891910265</v>
+        <v>0.668</v>
       </c>
       <c r="J81">
-        <v>0.5335365853658537</v>
+        <v>0.534</v>
       </c>
       <c r="K81">
-        <v>0.6926994906621392</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="L81">
-        <v>0.5355079850492694</v>
+        <v>0.536</v>
       </c>
       <c r="M81">
-        <v>0.3421588594704684</v>
+        <v>0.342</v>
       </c>
       <c r="N81">
-        <v>0.1357481381178064</v>
+        <v>0.136</v>
       </c>
     </row>
     <row r="82">
@@ -4120,40 +4120,40 @@
         <v>1999</v>
       </c>
       <c r="C82">
-        <v>0.9478924659807501</v>
+        <v>0.948</v>
       </c>
       <c r="D82">
-        <v>0.7758203799654577</v>
+        <v>0.776</v>
       </c>
       <c r="E82">
-        <v>0.7837370242214533</v>
+        <v>0.784</v>
       </c>
       <c r="F82">
-        <v>0.6537935748462064</v>
+        <v>0.654</v>
       </c>
       <c r="G82">
-        <v>0.7309523809523809</v>
+        <v>0.731</v>
       </c>
       <c r="H82">
-        <v>0.7981438515081206</v>
+        <v>0.798</v>
       </c>
       <c r="I82">
         <v>0.72</v>
       </c>
       <c r="J82">
-        <v>0.687131460284426</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="K82">
-        <v>0.62491559756921</v>
+        <v>0.625</v>
       </c>
       <c r="L82">
-        <v>0.5886681383370125</v>
+        <v>0.589</v>
       </c>
       <c r="M82">
-        <v>0.378191856452726</v>
+        <v>0.378</v>
       </c>
       <c r="N82">
-        <v>0.2943562014193984</v>
+        <v>0.294</v>
       </c>
     </row>
     <row r="83">
@@ -4166,40 +4166,40 @@
         <v>2009</v>
       </c>
       <c r="C83">
-        <v>0.9071452090879157</v>
+        <v>0.907</v>
       </c>
       <c r="D83">
-        <v>0.8073485600794439</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="E83">
-        <v>0.7491738268341044</v>
+        <v>0.749</v>
       </c>
       <c r="F83">
-        <v>0.7134849983514672</v>
+        <v>0.713</v>
       </c>
       <c r="G83">
-        <v>0.8242664029014177</v>
+        <v>0.824</v>
       </c>
       <c r="H83">
-        <v>0.7455621301775148</v>
+        <v>0.746</v>
       </c>
       <c r="I83">
-        <v>0.6601717305151915</v>
+        <v>0.66</v>
       </c>
       <c r="J83">
-        <v>0.7246042216358839</v>
+        <v>0.725</v>
       </c>
       <c r="K83">
-        <v>0.5702043506921556</v>
+        <v>0.57</v>
       </c>
       <c r="L83">
-        <v>0.5556656755863891</v>
+        <v>0.556</v>
       </c>
       <c r="M83">
-        <v>0.3439973614775725</v>
+        <v>0.344</v>
       </c>
       <c r="N83">
-        <v>0.2537018756169793</v>
+        <v>0.254</v>
       </c>
     </row>
     <row r="84">
@@ -4212,40 +4212,40 @@
         <v>2016</v>
       </c>
       <c r="C84">
-        <v>0.9199857752489331</v>
+        <v>0.92</v>
       </c>
       <c r="D84">
-        <v>0.8463180362860192</v>
+        <v>0.846</v>
       </c>
       <c r="E84">
-        <v>0.7949358059914408</v>
+        <v>0.795</v>
       </c>
       <c r="F84">
-        <v>0.8526165895336418</v>
+        <v>0.853</v>
       </c>
       <c r="G84">
-        <v>0.8557178482365515</v>
+        <v>0.856</v>
       </c>
       <c r="H84">
-        <v>0.7963944856839873</v>
+        <v>0.796</v>
       </c>
       <c r="I84">
-        <v>0.6846814602720115</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="J84">
-        <v>0.7608540925266903</v>
+        <v>0.761</v>
       </c>
       <c r="K84">
-        <v>0.6567164179104478</v>
+        <v>0.657</v>
       </c>
       <c r="L84">
-        <v>0.5693404634581105</v>
+        <v>0.569</v>
       </c>
       <c r="M84">
-        <v>0.4024346580737558</v>
+        <v>0.402</v>
       </c>
       <c r="N84">
-        <v>0.2613475177304965</v>
+        <v>0.261</v>
       </c>
     </row>
     <row r="85">
@@ -4258,40 +4258,40 @@
         <v>1999</v>
       </c>
       <c r="C85">
-        <v>0.9596532177392464</v>
+        <v>0.96</v>
       </c>
       <c r="D85">
-        <v>0.7816901408450704</v>
+        <v>0.782</v>
       </c>
       <c r="E85">
-        <v>0.8206106870229007</v>
+        <v>0.821</v>
       </c>
       <c r="F85">
-        <v>0.7841726618705036</v>
+        <v>0.784</v>
       </c>
       <c r="G85">
-        <v>0.806999306999307</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="H85">
-        <v>0.7922428330522766</v>
+        <v>0.792</v>
       </c>
       <c r="I85">
-        <v>0.6244870041039672</v>
+        <v>0.624</v>
       </c>
       <c r="J85">
-        <v>0.6427815037063184</v>
+        <v>0.643</v>
       </c>
       <c r="K85">
-        <v>0.5616580310880829</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="L85">
-        <v>0.6883636363636364</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="M85">
-        <v>0.3889479277364506</v>
+        <v>0.389</v>
       </c>
       <c r="N85">
-        <v>0.2114186851211073</v>
+        <v>0.211</v>
       </c>
     </row>
     <row r="86">
@@ -4304,40 +4304,40 @@
         <v>2009</v>
       </c>
       <c r="C86">
-        <v>0.8792085056113408</v>
+        <v>0.879</v>
       </c>
       <c r="D86">
-        <v>0.7608052101835405</v>
+        <v>0.761</v>
       </c>
       <c r="E86">
-        <v>0.7822104018912529</v>
+        <v>0.782</v>
       </c>
       <c r="F86">
-        <v>0.8229566243729713</v>
+        <v>0.823</v>
       </c>
       <c r="G86">
-        <v>0.8079646017699115</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="H86">
-        <v>0.7647058823529411</v>
+        <v>0.765</v>
       </c>
       <c r="I86">
-        <v>0.4511943379534061</v>
+        <v>0.451</v>
       </c>
       <c r="J86">
-        <v>0.8114826871855578</v>
+        <v>0.8110000000000001</v>
       </c>
       <c r="K86">
-        <v>0.6202830188679245</v>
+        <v>0.62</v>
       </c>
       <c r="L86">
-        <v>0.5948429164196799</v>
+        <v>0.595</v>
       </c>
       <c r="M86">
-        <v>0.3406333234684818</v>
+        <v>0.341</v>
       </c>
       <c r="N86">
-        <v>0.2272995283018868</v>
+        <v>0.227</v>
       </c>
     </row>
     <row r="87">
@@ -4350,40 +4350,40 @@
         <v>2016</v>
       </c>
       <c r="C87">
-        <v>0.9450303611377436</v>
+        <v>0.945</v>
       </c>
       <c r="D87">
-        <v>0.8214627914404343</v>
+        <v>0.821</v>
       </c>
       <c r="E87">
-        <v>0.8126598465473146</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="F87">
-        <v>0.8442179037910162</v>
+        <v>0.844</v>
       </c>
       <c r="G87">
-        <v>0.8383060635226179</v>
+        <v>0.838</v>
       </c>
       <c r="H87">
-        <v>0.8633207070707071</v>
+        <v>0.863</v>
       </c>
       <c r="I87">
-        <v>0.4833440102498399</v>
+        <v>0.483</v>
       </c>
       <c r="J87">
-        <v>0.8774588842308932</v>
+        <v>0.877</v>
       </c>
       <c r="K87">
-        <v>0.7314194577352472</v>
+        <v>0.731</v>
       </c>
       <c r="L87">
-        <v>0.65270227054685</v>
+        <v>0.653</v>
       </c>
       <c r="M87">
-        <v>0.4766025641025641</v>
+        <v>0.477</v>
       </c>
       <c r="N87">
-        <v>0.2199488491048593</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="88">
@@ -4396,40 +4396,40 @@
         <v>2009</v>
       </c>
       <c r="C88">
-        <v>0.9486445208094693</v>
+        <v>0.949</v>
       </c>
       <c r="D88">
-        <v>0.9261102603369066</v>
+        <v>0.926</v>
       </c>
       <c r="E88">
-        <v>0.9328358208955224</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="F88">
-        <v>0.5644945537932352</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="G88">
-        <v>0.949301702697532</v>
+        <v>0.949</v>
       </c>
       <c r="H88">
-        <v>0.9727255388136563</v>
+        <v>0.973</v>
       </c>
       <c r="I88">
-        <v>0.9295450182376656</v>
+        <v>0.93</v>
       </c>
       <c r="J88">
-        <v>0.8251146788990825</v>
+        <v>0.825</v>
       </c>
       <c r="K88">
-        <v>0.9111238532110092</v>
+        <v>0.911</v>
       </c>
       <c r="L88">
-        <v>0.6480489671002295</v>
+        <v>0.648</v>
       </c>
       <c r="M88">
-        <v>0.7105666156202144</v>
+        <v>0.711</v>
       </c>
       <c r="N88">
-        <v>0.6748947569843092</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="89">
@@ -4442,40 +4442,40 @@
         <v>2009</v>
       </c>
       <c r="C89">
-        <v>0.9634170071998444</v>
+        <v>0.963</v>
       </c>
       <c r="D89">
-        <v>0.9047340736411456</v>
+        <v>0.905</v>
       </c>
       <c r="E89">
-        <v>0.8897116134060795</v>
+        <v>0.89</v>
       </c>
       <c r="F89">
-        <v>0.9451041463889429</v>
+        <v>0.945</v>
       </c>
       <c r="G89">
-        <v>0.8872004675628288</v>
+        <v>0.887</v>
       </c>
       <c r="H89">
-        <v>0.7482966712088768</v>
+        <v>0.748</v>
       </c>
       <c r="I89">
-        <v>0.7900584795321638</v>
+        <v>0.79</v>
       </c>
       <c r="J89">
-        <v>0.7191273860537593</v>
+        <v>0.719</v>
       </c>
       <c r="K89">
-        <v>0.8743914313534566</v>
+        <v>0.874</v>
       </c>
       <c r="L89">
-        <v>0.6419103313840155</v>
+        <v>0.642</v>
       </c>
       <c r="M89">
-        <v>0.5105263157894737</v>
+        <v>0.511</v>
       </c>
       <c r="N89">
-        <v>0.1662772585669782</v>
+        <v>0.166</v>
       </c>
     </row>
     <row r="90">
@@ -4488,40 +4488,40 @@
         <v>2016</v>
       </c>
       <c r="C90">
-        <v>0.9802130898021308</v>
+        <v>0.98</v>
       </c>
       <c r="D90">
-        <v>0.8734145104008117</v>
+        <v>0.873</v>
       </c>
       <c r="E90">
-        <v>0.8688815622622369</v>
+        <v>0.869</v>
       </c>
       <c r="F90">
-        <v>0.943683409436834</v>
+        <v>0.944</v>
       </c>
       <c r="G90">
-        <v>0.8929205785333671</v>
+        <v>0.893</v>
       </c>
       <c r="H90">
-        <v>0.7793558204412884</v>
+        <v>0.779</v>
       </c>
       <c r="I90">
-        <v>0.818089430894309</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="J90">
-        <v>0.7716315655924892</v>
+        <v>0.772</v>
       </c>
       <c r="K90">
-        <v>0.8985544002028912</v>
+        <v>0.899</v>
       </c>
       <c r="L90">
-        <v>0.6809753619507239</v>
+        <v>0.681</v>
       </c>
       <c r="M90">
-        <v>0.5946700507614213</v>
+        <v>0.595</v>
       </c>
       <c r="N90">
-        <v>0.2106598984771574</v>
+        <v>0.211</v>
       </c>
     </row>
     <row r="91">
@@ -4534,40 +4534,40 @@
         <v>1999</v>
       </c>
       <c r="C91">
-        <v>0.952082565425728</v>
+        <v>0.952</v>
       </c>
       <c r="D91">
-        <v>0.8316679477325134</v>
+        <v>0.832</v>
       </c>
       <c r="E91">
-        <v>0.8808988764044944</v>
+        <v>0.881</v>
       </c>
       <c r="F91">
-        <v>0.9123134328358209</v>
+        <v>0.912</v>
       </c>
       <c r="G91">
-        <v>0.8316190476190476</v>
+        <v>0.832</v>
       </c>
       <c r="H91">
-        <v>0.8303571428571429</v>
+        <v>0.83</v>
       </c>
       <c r="I91">
-        <v>0.7301168488503581</v>
+        <v>0.73</v>
       </c>
       <c r="J91">
-        <v>0.7950169875424689</v>
+        <v>0.795</v>
       </c>
       <c r="K91">
-        <v>0.6398013750954927</v>
+        <v>0.64</v>
       </c>
       <c r="L91">
-        <v>0.7223127035830619</v>
+        <v>0.722</v>
       </c>
       <c r="M91">
-        <v>0.5806709265175719</v>
+        <v>0.581</v>
       </c>
       <c r="N91">
-        <v>0.4737460815047022</v>
+        <v>0.474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ICCS ran new code
</commit_message>
<xml_diff>
--- a/clean-data/output/citizenship-norm-indicator-tables.xlsx
+++ b/clean-data/output/citizenship-norm-indicator-tables.xlsx
@@ -440,7 +440,7 @@
         <v>1999</v>
       </c>
       <c r="C2">
-        <v>0.929</v>
+        <v>0.9290000000000001</v>
       </c>
       <c r="D2">
         <v>0.6870000000000001</v>
@@ -507,7 +507,7 @@
         <v>0.772</v>
       </c>
       <c r="J3">
-        <v>0.679</v>
+        <v>0.6790000000000001</v>
       </c>
       <c r="K3">
         <v>0.6870000000000001</v>
@@ -581,10 +581,10 @@
         <v>0.9340000000000001</v>
       </c>
       <c r="D5">
-        <v>0.8139999999999999</v>
+        <v>0.814</v>
       </c>
       <c r="E5">
-        <v>0.804</v>
+        <v>0.8040000000000001</v>
       </c>
       <c r="F5">
         <v>0.863</v>
@@ -596,7 +596,7 @@
         <v>0.846</v>
       </c>
       <c r="I5">
-        <v>0.5679999999999999</v>
+        <v>0.568</v>
       </c>
       <c r="J5">
         <v>0.879</v>
@@ -639,19 +639,19 @@
         <v>0.72</v>
       </c>
       <c r="H6">
-        <v>0.8149999999999999</v>
+        <v>0.815</v>
       </c>
       <c r="I6">
         <v>0.419</v>
       </c>
       <c r="J6">
-        <v>0.555</v>
+        <v>0.5550000000000001</v>
       </c>
       <c r="K6">
         <v>0.579</v>
       </c>
       <c r="L6">
-        <v>0.5639999999999999</v>
+        <v>0.564</v>
       </c>
       <c r="M6">
         <v>0.387</v>
@@ -676,13 +676,13 @@
         <v>0.823</v>
       </c>
       <c r="E7">
-        <v>0.677</v>
+        <v>0.6770000000000001</v>
       </c>
       <c r="F7">
-        <v>0.8159999999999999</v>
+        <v>0.816</v>
       </c>
       <c r="G7">
-        <v>0.8149999999999999</v>
+        <v>0.815</v>
       </c>
       <c r="H7">
         <v>0.707</v>
@@ -691,10 +691,10 @@
         <v>0.799</v>
       </c>
       <c r="J7">
-        <v>0.676</v>
+        <v>0.6760000000000001</v>
       </c>
       <c r="K7">
-        <v>0.676</v>
+        <v>0.6760000000000001</v>
       </c>
       <c r="L7">
         <v>0.709</v>
@@ -955,7 +955,7 @@
         <v>0.903</v>
       </c>
       <c r="F13">
-        <v>0.804</v>
+        <v>0.8040000000000001</v>
       </c>
       <c r="G13">
         <v>0.903</v>
@@ -970,7 +970,7 @@
         <v>0.849</v>
       </c>
       <c r="K13">
-        <v>0.677</v>
+        <v>0.6770000000000001</v>
       </c>
       <c r="L13">
         <v>0.661</v>
@@ -1041,16 +1041,16 @@
         <v>0.974</v>
       </c>
       <c r="D15">
-        <v>0.9409999999999999</v>
+        <v>0.941</v>
       </c>
       <c r="E15">
-        <v>0.9419999999999999</v>
+        <v>0.942</v>
       </c>
       <c r="F15">
         <v>0.837</v>
       </c>
       <c r="G15">
-        <v>0.9389999999999999</v>
+        <v>0.939</v>
       </c>
       <c r="H15">
         <v>0.879</v>
@@ -1087,7 +1087,7 @@
         <v>0.875</v>
       </c>
       <c r="D16">
-        <v>0.9409999999999999</v>
+        <v>0.941</v>
       </c>
       <c r="E16">
         <v>0.898</v>
@@ -1194,7 +1194,7 @@
         <v>0.914</v>
       </c>
       <c r="I18">
-        <v>0.926</v>
+        <v>0.9260000000000001</v>
       </c>
       <c r="J18">
         <v>0.909</v>
@@ -1234,7 +1234,7 @@
         <v>0.718</v>
       </c>
       <c r="G19">
-        <v>0.805</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="H19">
         <v>0.821</v>
@@ -1280,10 +1280,10 @@
         <v>0.772</v>
       </c>
       <c r="G20">
-        <v>0.8159999999999999</v>
+        <v>0.816</v>
       </c>
       <c r="H20">
-        <v>0.68</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="I20">
         <v>0.716</v>
@@ -1317,7 +1317,7 @@
         <v>0.922</v>
       </c>
       <c r="D21">
-        <v>0.8169999999999999</v>
+        <v>0.817</v>
       </c>
       <c r="E21">
         <v>0.767</v>
@@ -1452,13 +1452,13 @@
         <v>2009</v>
       </c>
       <c r="C24">
-        <v>0.9429999999999999</v>
+        <v>0.943</v>
       </c>
       <c r="D24">
         <v>0.6879999999999999</v>
       </c>
       <c r="E24">
-        <v>0.554</v>
+        <v>0.5540000000000001</v>
       </c>
       <c r="F24">
         <v>0.75</v>
@@ -1470,7 +1470,7 @@
         <v>0.791</v>
       </c>
       <c r="I24">
-        <v>0.677</v>
+        <v>0.6770000000000001</v>
       </c>
       <c r="J24">
         <v>0.883</v>
@@ -1636,7 +1636,7 @@
         <v>2016</v>
       </c>
       <c r="C28">
-        <v>0.9389999999999999</v>
+        <v>0.939</v>
       </c>
       <c r="D28">
         <v>0.919</v>
@@ -1654,7 +1654,7 @@
         <v>0.77</v>
       </c>
       <c r="I28">
-        <v>0.9429999999999999</v>
+        <v>0.943</v>
       </c>
       <c r="J28">
         <v>0.916</v>
@@ -1691,7 +1691,7 @@
         <v>0.785</v>
       </c>
       <c r="F29">
-        <v>0.927</v>
+        <v>0.9270000000000001</v>
       </c>
       <c r="G29">
         <v>0.763</v>
@@ -1749,7 +1749,7 @@
         <v>0.628</v>
       </c>
       <c r="J30">
-        <v>0.801</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="K30">
         <v>0.712</v>
@@ -1792,7 +1792,7 @@
         <v>0.761</v>
       </c>
       <c r="I31">
-        <v>0.6889999999999999</v>
+        <v>0.689</v>
       </c>
       <c r="J31">
         <v>0.787</v>
@@ -1832,7 +1832,7 @@
         <v>0.827</v>
       </c>
       <c r="G32">
-        <v>0.681</v>
+        <v>0.6810000000000001</v>
       </c>
       <c r="H32">
         <v>0.701</v>
@@ -1884,7 +1884,7 @@
         <v>0.669</v>
       </c>
       <c r="I33">
-        <v>0.805</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="J33">
         <v>0.731</v>
@@ -2111,7 +2111,7 @@
         <v>0.888</v>
       </c>
       <c r="H38">
-        <v>0.9429999999999999</v>
+        <v>0.943</v>
       </c>
       <c r="I38">
         <v>0.881</v>
@@ -2160,7 +2160,7 @@
         <v>0.747</v>
       </c>
       <c r="I39">
-        <v>0.8179999999999999</v>
+        <v>0.818</v>
       </c>
       <c r="J39">
         <v>0.718</v>
@@ -2172,7 +2172,7 @@
         <v>0.778</v>
       </c>
       <c r="M39">
-        <v>0.5679999999999999</v>
+        <v>0.568</v>
       </c>
       <c r="N39">
         <v>0.267</v>
@@ -2206,7 +2206,7 @@
         <v>0.922</v>
       </c>
       <c r="I40">
-        <v>0.926</v>
+        <v>0.9260000000000001</v>
       </c>
       <c r="J40">
         <v>0.9</v>
@@ -2237,7 +2237,7 @@
         <v>0.944</v>
       </c>
       <c r="D41">
-        <v>0.801</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="E41">
         <v>0.852</v>
@@ -2326,7 +2326,7 @@
         <v>2016</v>
       </c>
       <c r="C43">
-        <v>0.93</v>
+        <v>0.9300000000000001</v>
       </c>
       <c r="D43">
         <v>0.773</v>
@@ -2372,7 +2372,7 @@
         <v>2016</v>
       </c>
       <c r="C44">
-        <v>0.9419999999999999</v>
+        <v>0.942</v>
       </c>
       <c r="D44">
         <v>0.907</v>
@@ -2384,7 +2384,7 @@
         <v>0.953</v>
       </c>
       <c r="G44">
-        <v>0.927</v>
+        <v>0.9270000000000001</v>
       </c>
       <c r="H44">
         <v>0.9</v>
@@ -2433,7 +2433,7 @@
         <v>0.765</v>
       </c>
       <c r="H45">
-        <v>0.8149999999999999</v>
+        <v>0.815</v>
       </c>
       <c r="I45">
         <v>0.858</v>
@@ -2470,10 +2470,10 @@
         <v>0.857</v>
       </c>
       <c r="E46">
-        <v>0.931</v>
+        <v>0.9310000000000001</v>
       </c>
       <c r="F46">
-        <v>0.9389999999999999</v>
+        <v>0.939</v>
       </c>
       <c r="G46">
         <v>0.9360000000000001</v>
@@ -2491,13 +2491,13 @@
         <v>0.743</v>
       </c>
       <c r="L46">
-        <v>0.806</v>
+        <v>0.8060000000000001</v>
       </c>
       <c r="M46">
         <v>0.482</v>
       </c>
       <c r="N46">
-        <v>0.551</v>
+        <v>0.5510000000000001</v>
       </c>
     </row>
     <row r="47">
@@ -2666,7 +2666,7 @@
         <v>0.91</v>
       </c>
       <c r="I50">
-        <v>0.928</v>
+        <v>0.9280000000000001</v>
       </c>
       <c r="J50">
         <v>0.828</v>
@@ -2740,7 +2740,7 @@
         <v>2016</v>
       </c>
       <c r="C52">
-        <v>0.9389999999999999</v>
+        <v>0.939</v>
       </c>
       <c r="D52">
         <v>0.836</v>
@@ -2755,7 +2755,7 @@
         <v>0.898</v>
       </c>
       <c r="H52">
-        <v>0.926</v>
+        <v>0.9260000000000001</v>
       </c>
       <c r="I52">
         <v>0.821</v>
@@ -2792,7 +2792,7 @@
         <v>0.714</v>
       </c>
       <c r="E53">
-        <v>0.681</v>
+        <v>0.6810000000000001</v>
       </c>
       <c r="F53">
         <v>0.626</v>
@@ -2801,7 +2801,7 @@
         <v>0.652</v>
       </c>
       <c r="H53">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="I53">
         <v>0.754</v>
@@ -2832,7 +2832,7 @@
         <v>1999</v>
       </c>
       <c r="C54">
-        <v>0.928</v>
+        <v>0.9280000000000001</v>
       </c>
       <c r="D54">
         <v>0.903</v>
@@ -2850,7 +2850,7 @@
         <v>0.839</v>
       </c>
       <c r="I54">
-        <v>0.806</v>
+        <v>0.8060000000000001</v>
       </c>
       <c r="J54">
         <v>0.76</v>
@@ -2862,7 +2862,7 @@
         <v>0.721</v>
       </c>
       <c r="M54">
-        <v>0.5649999999999999</v>
+        <v>0.565</v>
       </c>
       <c r="N54">
         <v>0.387</v>
@@ -2884,7 +2884,7 @@
         <v>0.765</v>
       </c>
       <c r="E55">
-        <v>0.8149999999999999</v>
+        <v>0.815</v>
       </c>
       <c r="F55">
         <v>0.745</v>
@@ -2893,7 +2893,7 @@
         <v>0.771</v>
       </c>
       <c r="H55">
-        <v>0.806</v>
+        <v>0.8060000000000001</v>
       </c>
       <c r="I55">
         <v>0.891</v>
@@ -2924,7 +2924,7 @@
         <v>2016</v>
       </c>
       <c r="C56">
-        <v>0.931</v>
+        <v>0.9310000000000001</v>
       </c>
       <c r="D56">
         <v>0.754</v>
@@ -2979,7 +2979,7 @@
         <v>0.665</v>
       </c>
       <c r="F57">
-        <v>0.679</v>
+        <v>0.6790000000000001</v>
       </c>
       <c r="G57">
         <v>0.748</v>
@@ -3025,7 +3025,7 @@
         <v>0.726</v>
       </c>
       <c r="F58">
-        <v>0.801</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="G58">
         <v>0.761</v>
@@ -3126,10 +3126,10 @@
         <v>0.791</v>
       </c>
       <c r="I60">
-        <v>0.805</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="J60">
-        <v>0.8169999999999999</v>
+        <v>0.817</v>
       </c>
       <c r="K60">
         <v>0.785</v>
@@ -3172,7 +3172,7 @@
         <v>0.87</v>
       </c>
       <c r="I61">
-        <v>0.8159999999999999</v>
+        <v>0.816</v>
       </c>
       <c r="J61">
         <v>0.784</v>
@@ -3298,7 +3298,7 @@
         <v>0.849</v>
       </c>
       <c r="E64">
-        <v>0.803</v>
+        <v>0.8030000000000001</v>
       </c>
       <c r="F64">
         <v>0.834</v>
@@ -3359,7 +3359,7 @@
         <v>0.46</v>
       </c>
       <c r="J65">
-        <v>0.805</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="K65">
         <v>0.668</v>
@@ -3457,7 +3457,7 @@
         <v>0.671</v>
       </c>
       <c r="L67">
-        <v>0.676</v>
+        <v>0.6760000000000001</v>
       </c>
       <c r="M67">
         <v>0.362</v>
@@ -3500,7 +3500,7 @@
         <v>0.86</v>
       </c>
       <c r="K68">
-        <v>0.801</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="L68">
         <v>0.697</v>
@@ -3522,7 +3522,7 @@
         <v>2016</v>
       </c>
       <c r="C69">
-        <v>0.928</v>
+        <v>0.9280000000000001</v>
       </c>
       <c r="D69">
         <v>0.8110000000000001</v>
@@ -3592,7 +3592,7 @@
         <v>0.788</v>
       </c>
       <c r="K70">
-        <v>0.6919999999999999</v>
+        <v>0.692</v>
       </c>
       <c r="L70">
         <v>0.529</v>
@@ -3632,7 +3632,7 @@
         <v>0.951</v>
       </c>
       <c r="I71">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="J71">
         <v>0.92</v>
@@ -3663,7 +3663,7 @@
         <v>0.961</v>
       </c>
       <c r="D72">
-        <v>0.8169999999999999</v>
+        <v>0.817</v>
       </c>
       <c r="E72">
         <v>0.907</v>
@@ -3681,7 +3681,7 @@
         <v>0.898</v>
       </c>
       <c r="J72">
-        <v>0.8159999999999999</v>
+        <v>0.816</v>
       </c>
       <c r="K72">
         <v>0.861</v>
@@ -3690,7 +3690,7 @@
         <v>0.766</v>
       </c>
       <c r="M72">
-        <v>0.553</v>
+        <v>0.5530000000000001</v>
       </c>
       <c r="N72">
         <v>0.387</v>
@@ -3718,7 +3718,7 @@
         <v>0.641</v>
       </c>
       <c r="G73">
-        <v>0.8169999999999999</v>
+        <v>0.817</v>
       </c>
       <c r="H73">
         <v>0.891</v>
@@ -3758,10 +3758,10 @@
         <v>0.883</v>
       </c>
       <c r="E74">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="F74">
-        <v>0.8159999999999999</v>
+        <v>0.816</v>
       </c>
       <c r="G74">
         <v>0.921</v>
@@ -3776,7 +3776,7 @@
         <v>0.828</v>
       </c>
       <c r="K74">
-        <v>0.8149999999999999</v>
+        <v>0.815</v>
       </c>
       <c r="L74">
         <v>0.734</v>
@@ -3871,7 +3871,7 @@
         <v>0.782</v>
       </c>
       <c r="L76">
-        <v>0.68</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="M76">
         <v>0.5629999999999999</v>
@@ -3902,7 +3902,7 @@
         <v>0.887</v>
       </c>
       <c r="G77">
-        <v>0.802</v>
+        <v>0.8020000000000001</v>
       </c>
       <c r="H77">
         <v>0.791</v>
@@ -3942,7 +3942,7 @@
         <v>0.827</v>
       </c>
       <c r="E78">
-        <v>0.801</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="F78">
         <v>0.821</v>
@@ -3960,10 +3960,10 @@
         <v>0.849</v>
       </c>
       <c r="K78">
-        <v>0.805</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="L78">
-        <v>0.68</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="M78">
         <v>0.454</v>
@@ -3988,7 +3988,7 @@
         <v>0.8080000000000001</v>
       </c>
       <c r="E79">
-        <v>0.8139999999999999</v>
+        <v>0.814</v>
       </c>
       <c r="F79">
         <v>0.836</v>
@@ -4031,7 +4031,7 @@
         <v>0.985</v>
       </c>
       <c r="D80">
-        <v>0.931</v>
+        <v>0.9310000000000001</v>
       </c>
       <c r="E80">
         <v>0.872</v>
@@ -4098,7 +4098,7 @@
         <v>0.534</v>
       </c>
       <c r="K81">
-        <v>0.6929999999999999</v>
+        <v>0.693</v>
       </c>
       <c r="L81">
         <v>0.536</v>
@@ -4193,7 +4193,7 @@
         <v>0.57</v>
       </c>
       <c r="L83">
-        <v>0.556</v>
+        <v>0.5560000000000001</v>
       </c>
       <c r="M83">
         <v>0.344</v>
@@ -4399,13 +4399,13 @@
         <v>0.949</v>
       </c>
       <c r="D88">
-        <v>0.926</v>
+        <v>0.9260000000000001</v>
       </c>
       <c r="E88">
         <v>0.9330000000000001</v>
       </c>
       <c r="F88">
-        <v>0.5639999999999999</v>
+        <v>0.564</v>
       </c>
       <c r="G88">
         <v>0.949</v>
@@ -4414,7 +4414,7 @@
         <v>0.973</v>
       </c>
       <c r="I88">
-        <v>0.93</v>
+        <v>0.9300000000000001</v>
       </c>
       <c r="J88">
         <v>0.825</v>
@@ -4506,7 +4506,7 @@
         <v>0.779</v>
       </c>
       <c r="I90">
-        <v>0.8179999999999999</v>
+        <v>0.818</v>
       </c>
       <c r="J90">
         <v>0.772</v>
@@ -4515,7 +4515,7 @@
         <v>0.899</v>
       </c>
       <c r="L90">
-        <v>0.681</v>
+        <v>0.6810000000000001</v>
       </c>
       <c r="M90">
         <v>0.595</v>

</xml_diff>

<commit_message>
Ran new recoded control vars & knitr
</commit_message>
<xml_diff>
--- a/clean-data/output/citizenship-norm-indicator-tables.xlsx
+++ b/clean-data/output/citizenship-norm-indicator-tables.xlsx
@@ -440,7 +440,7 @@
         <v>1999</v>
       </c>
       <c r="C2">
-        <v>0.929</v>
+        <v>0.9290000000000001</v>
       </c>
       <c r="D2">
         <v>0.6870000000000001</v>
@@ -507,7 +507,7 @@
         <v>0.772</v>
       </c>
       <c r="J3">
-        <v>0.679</v>
+        <v>0.6790000000000001</v>
       </c>
       <c r="K3">
         <v>0.6870000000000001</v>
@@ -581,10 +581,10 @@
         <v>0.9340000000000001</v>
       </c>
       <c r="D5">
-        <v>0.8139999999999999</v>
+        <v>0.814</v>
       </c>
       <c r="E5">
-        <v>0.804</v>
+        <v>0.8040000000000001</v>
       </c>
       <c r="F5">
         <v>0.863</v>
@@ -596,7 +596,7 @@
         <v>0.846</v>
       </c>
       <c r="I5">
-        <v>0.5679999999999999</v>
+        <v>0.568</v>
       </c>
       <c r="J5">
         <v>0.879</v>
@@ -639,19 +639,19 @@
         <v>0.72</v>
       </c>
       <c r="H6">
-        <v>0.8149999999999999</v>
+        <v>0.815</v>
       </c>
       <c r="I6">
         <v>0.419</v>
       </c>
       <c r="J6">
-        <v>0.555</v>
+        <v>0.5550000000000001</v>
       </c>
       <c r="K6">
         <v>0.579</v>
       </c>
       <c r="L6">
-        <v>0.5639999999999999</v>
+        <v>0.564</v>
       </c>
       <c r="M6">
         <v>0.387</v>
@@ -676,13 +676,13 @@
         <v>0.823</v>
       </c>
       <c r="E7">
-        <v>0.677</v>
+        <v>0.6770000000000001</v>
       </c>
       <c r="F7">
-        <v>0.8159999999999999</v>
+        <v>0.816</v>
       </c>
       <c r="G7">
-        <v>0.8149999999999999</v>
+        <v>0.815</v>
       </c>
       <c r="H7">
         <v>0.707</v>
@@ -691,10 +691,10 @@
         <v>0.799</v>
       </c>
       <c r="J7">
-        <v>0.676</v>
+        <v>0.6760000000000001</v>
       </c>
       <c r="K7">
-        <v>0.676</v>
+        <v>0.6760000000000001</v>
       </c>
       <c r="L7">
         <v>0.709</v>
@@ -955,7 +955,7 @@
         <v>0.903</v>
       </c>
       <c r="F13">
-        <v>0.804</v>
+        <v>0.8040000000000001</v>
       </c>
       <c r="G13">
         <v>0.903</v>
@@ -970,7 +970,7 @@
         <v>0.849</v>
       </c>
       <c r="K13">
-        <v>0.677</v>
+        <v>0.6770000000000001</v>
       </c>
       <c r="L13">
         <v>0.661</v>
@@ -1041,16 +1041,16 @@
         <v>0.974</v>
       </c>
       <c r="D15">
-        <v>0.9409999999999999</v>
+        <v>0.941</v>
       </c>
       <c r="E15">
-        <v>0.9419999999999999</v>
+        <v>0.942</v>
       </c>
       <c r="F15">
         <v>0.837</v>
       </c>
       <c r="G15">
-        <v>0.9389999999999999</v>
+        <v>0.939</v>
       </c>
       <c r="H15">
         <v>0.879</v>
@@ -1087,7 +1087,7 @@
         <v>0.875</v>
       </c>
       <c r="D16">
-        <v>0.9409999999999999</v>
+        <v>0.941</v>
       </c>
       <c r="E16">
         <v>0.898</v>
@@ -1194,7 +1194,7 @@
         <v>0.914</v>
       </c>
       <c r="I18">
-        <v>0.926</v>
+        <v>0.9260000000000001</v>
       </c>
       <c r="J18">
         <v>0.909</v>
@@ -1234,7 +1234,7 @@
         <v>0.718</v>
       </c>
       <c r="G19">
-        <v>0.805</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="H19">
         <v>0.821</v>
@@ -1280,10 +1280,10 @@
         <v>0.772</v>
       </c>
       <c r="G20">
-        <v>0.8159999999999999</v>
+        <v>0.816</v>
       </c>
       <c r="H20">
-        <v>0.68</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="I20">
         <v>0.716</v>
@@ -1317,7 +1317,7 @@
         <v>0.922</v>
       </c>
       <c r="D21">
-        <v>0.8169999999999999</v>
+        <v>0.817</v>
       </c>
       <c r="E21">
         <v>0.767</v>
@@ -1452,13 +1452,13 @@
         <v>2009</v>
       </c>
       <c r="C24">
-        <v>0.9429999999999999</v>
+        <v>0.943</v>
       </c>
       <c r="D24">
         <v>0.6879999999999999</v>
       </c>
       <c r="E24">
-        <v>0.554</v>
+        <v>0.5540000000000001</v>
       </c>
       <c r="F24">
         <v>0.75</v>
@@ -1470,7 +1470,7 @@
         <v>0.791</v>
       </c>
       <c r="I24">
-        <v>0.677</v>
+        <v>0.6770000000000001</v>
       </c>
       <c r="J24">
         <v>0.883</v>
@@ -1636,7 +1636,7 @@
         <v>2016</v>
       </c>
       <c r="C28">
-        <v>0.9389999999999999</v>
+        <v>0.939</v>
       </c>
       <c r="D28">
         <v>0.919</v>
@@ -1654,7 +1654,7 @@
         <v>0.77</v>
       </c>
       <c r="I28">
-        <v>0.9429999999999999</v>
+        <v>0.943</v>
       </c>
       <c r="J28">
         <v>0.916</v>
@@ -1691,7 +1691,7 @@
         <v>0.785</v>
       </c>
       <c r="F29">
-        <v>0.927</v>
+        <v>0.9270000000000001</v>
       </c>
       <c r="G29">
         <v>0.763</v>
@@ -1749,7 +1749,7 @@
         <v>0.628</v>
       </c>
       <c r="J30">
-        <v>0.801</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="K30">
         <v>0.712</v>
@@ -1792,7 +1792,7 @@
         <v>0.761</v>
       </c>
       <c r="I31">
-        <v>0.6889999999999999</v>
+        <v>0.689</v>
       </c>
       <c r="J31">
         <v>0.787</v>
@@ -1832,7 +1832,7 @@
         <v>0.827</v>
       </c>
       <c r="G32">
-        <v>0.681</v>
+        <v>0.6810000000000001</v>
       </c>
       <c r="H32">
         <v>0.701</v>
@@ -1884,7 +1884,7 @@
         <v>0.669</v>
       </c>
       <c r="I33">
-        <v>0.805</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="J33">
         <v>0.731</v>
@@ -2111,7 +2111,7 @@
         <v>0.888</v>
       </c>
       <c r="H38">
-        <v>0.9429999999999999</v>
+        <v>0.943</v>
       </c>
       <c r="I38">
         <v>0.881</v>
@@ -2160,7 +2160,7 @@
         <v>0.747</v>
       </c>
       <c r="I39">
-        <v>0.8179999999999999</v>
+        <v>0.818</v>
       </c>
       <c r="J39">
         <v>0.718</v>
@@ -2172,7 +2172,7 @@
         <v>0.778</v>
       </c>
       <c r="M39">
-        <v>0.5679999999999999</v>
+        <v>0.568</v>
       </c>
       <c r="N39">
         <v>0.267</v>
@@ -2206,7 +2206,7 @@
         <v>0.922</v>
       </c>
       <c r="I40">
-        <v>0.926</v>
+        <v>0.9260000000000001</v>
       </c>
       <c r="J40">
         <v>0.9</v>
@@ -2237,7 +2237,7 @@
         <v>0.944</v>
       </c>
       <c r="D41">
-        <v>0.801</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="E41">
         <v>0.852</v>
@@ -2326,7 +2326,7 @@
         <v>2016</v>
       </c>
       <c r="C43">
-        <v>0.93</v>
+        <v>0.9300000000000001</v>
       </c>
       <c r="D43">
         <v>0.773</v>
@@ -2372,7 +2372,7 @@
         <v>2016</v>
       </c>
       <c r="C44">
-        <v>0.9419999999999999</v>
+        <v>0.942</v>
       </c>
       <c r="D44">
         <v>0.907</v>
@@ -2384,7 +2384,7 @@
         <v>0.953</v>
       </c>
       <c r="G44">
-        <v>0.927</v>
+        <v>0.9270000000000001</v>
       </c>
       <c r="H44">
         <v>0.9</v>
@@ -2433,7 +2433,7 @@
         <v>0.765</v>
       </c>
       <c r="H45">
-        <v>0.8149999999999999</v>
+        <v>0.815</v>
       </c>
       <c r="I45">
         <v>0.858</v>
@@ -2470,10 +2470,10 @@
         <v>0.857</v>
       </c>
       <c r="E46">
-        <v>0.931</v>
+        <v>0.9310000000000001</v>
       </c>
       <c r="F46">
-        <v>0.9389999999999999</v>
+        <v>0.939</v>
       </c>
       <c r="G46">
         <v>0.9360000000000001</v>
@@ -2491,13 +2491,13 @@
         <v>0.743</v>
       </c>
       <c r="L46">
-        <v>0.806</v>
+        <v>0.8060000000000001</v>
       </c>
       <c r="M46">
         <v>0.482</v>
       </c>
       <c r="N46">
-        <v>0.551</v>
+        <v>0.5510000000000001</v>
       </c>
     </row>
     <row r="47">
@@ -2666,7 +2666,7 @@
         <v>0.91</v>
       </c>
       <c r="I50">
-        <v>0.928</v>
+        <v>0.9280000000000001</v>
       </c>
       <c r="J50">
         <v>0.828</v>
@@ -2740,7 +2740,7 @@
         <v>2016</v>
       </c>
       <c r="C52">
-        <v>0.9389999999999999</v>
+        <v>0.939</v>
       </c>
       <c r="D52">
         <v>0.836</v>
@@ -2755,7 +2755,7 @@
         <v>0.898</v>
       </c>
       <c r="H52">
-        <v>0.926</v>
+        <v>0.9260000000000001</v>
       </c>
       <c r="I52">
         <v>0.821</v>
@@ -2792,7 +2792,7 @@
         <v>0.714</v>
       </c>
       <c r="E53">
-        <v>0.681</v>
+        <v>0.6810000000000001</v>
       </c>
       <c r="F53">
         <v>0.626</v>
@@ -2801,7 +2801,7 @@
         <v>0.652</v>
       </c>
       <c r="H53">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="I53">
         <v>0.754</v>
@@ -2832,7 +2832,7 @@
         <v>1999</v>
       </c>
       <c r="C54">
-        <v>0.928</v>
+        <v>0.9280000000000001</v>
       </c>
       <c r="D54">
         <v>0.903</v>
@@ -2850,7 +2850,7 @@
         <v>0.839</v>
       </c>
       <c r="I54">
-        <v>0.806</v>
+        <v>0.8060000000000001</v>
       </c>
       <c r="J54">
         <v>0.76</v>
@@ -2862,7 +2862,7 @@
         <v>0.721</v>
       </c>
       <c r="M54">
-        <v>0.5649999999999999</v>
+        <v>0.565</v>
       </c>
       <c r="N54">
         <v>0.387</v>
@@ -2884,7 +2884,7 @@
         <v>0.765</v>
       </c>
       <c r="E55">
-        <v>0.8149999999999999</v>
+        <v>0.815</v>
       </c>
       <c r="F55">
         <v>0.745</v>
@@ -2893,7 +2893,7 @@
         <v>0.771</v>
       </c>
       <c r="H55">
-        <v>0.806</v>
+        <v>0.8060000000000001</v>
       </c>
       <c r="I55">
         <v>0.891</v>
@@ -2924,7 +2924,7 @@
         <v>2016</v>
       </c>
       <c r="C56">
-        <v>0.931</v>
+        <v>0.9310000000000001</v>
       </c>
       <c r="D56">
         <v>0.754</v>
@@ -2979,7 +2979,7 @@
         <v>0.665</v>
       </c>
       <c r="F57">
-        <v>0.679</v>
+        <v>0.6790000000000001</v>
       </c>
       <c r="G57">
         <v>0.748</v>
@@ -3025,7 +3025,7 @@
         <v>0.726</v>
       </c>
       <c r="F58">
-        <v>0.801</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="G58">
         <v>0.761</v>
@@ -3126,10 +3126,10 @@
         <v>0.791</v>
       </c>
       <c r="I60">
-        <v>0.805</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="J60">
-        <v>0.8169999999999999</v>
+        <v>0.817</v>
       </c>
       <c r="K60">
         <v>0.785</v>
@@ -3172,7 +3172,7 @@
         <v>0.87</v>
       </c>
       <c r="I61">
-        <v>0.8159999999999999</v>
+        <v>0.816</v>
       </c>
       <c r="J61">
         <v>0.784</v>
@@ -3298,7 +3298,7 @@
         <v>0.849</v>
       </c>
       <c r="E64">
-        <v>0.803</v>
+        <v>0.8030000000000001</v>
       </c>
       <c r="F64">
         <v>0.834</v>
@@ -3359,7 +3359,7 @@
         <v>0.46</v>
       </c>
       <c r="J65">
-        <v>0.805</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="K65">
         <v>0.668</v>
@@ -3457,7 +3457,7 @@
         <v>0.671</v>
       </c>
       <c r="L67">
-        <v>0.676</v>
+        <v>0.6760000000000001</v>
       </c>
       <c r="M67">
         <v>0.362</v>
@@ -3500,7 +3500,7 @@
         <v>0.86</v>
       </c>
       <c r="K68">
-        <v>0.801</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="L68">
         <v>0.697</v>
@@ -3522,7 +3522,7 @@
         <v>2016</v>
       </c>
       <c r="C69">
-        <v>0.928</v>
+        <v>0.9280000000000001</v>
       </c>
       <c r="D69">
         <v>0.8110000000000001</v>
@@ -3592,7 +3592,7 @@
         <v>0.788</v>
       </c>
       <c r="K70">
-        <v>0.6919999999999999</v>
+        <v>0.692</v>
       </c>
       <c r="L70">
         <v>0.529</v>
@@ -3632,7 +3632,7 @@
         <v>0.951</v>
       </c>
       <c r="I71">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="J71">
         <v>0.92</v>
@@ -3663,7 +3663,7 @@
         <v>0.961</v>
       </c>
       <c r="D72">
-        <v>0.8169999999999999</v>
+        <v>0.817</v>
       </c>
       <c r="E72">
         <v>0.907</v>
@@ -3681,7 +3681,7 @@
         <v>0.898</v>
       </c>
       <c r="J72">
-        <v>0.8159999999999999</v>
+        <v>0.816</v>
       </c>
       <c r="K72">
         <v>0.861</v>
@@ -3690,7 +3690,7 @@
         <v>0.766</v>
       </c>
       <c r="M72">
-        <v>0.553</v>
+        <v>0.5530000000000001</v>
       </c>
       <c r="N72">
         <v>0.387</v>
@@ -3718,7 +3718,7 @@
         <v>0.641</v>
       </c>
       <c r="G73">
-        <v>0.8169999999999999</v>
+        <v>0.817</v>
       </c>
       <c r="H73">
         <v>0.891</v>
@@ -3758,10 +3758,10 @@
         <v>0.883</v>
       </c>
       <c r="E74">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="F74">
-        <v>0.8159999999999999</v>
+        <v>0.816</v>
       </c>
       <c r="G74">
         <v>0.921</v>
@@ -3776,7 +3776,7 @@
         <v>0.828</v>
       </c>
       <c r="K74">
-        <v>0.8149999999999999</v>
+        <v>0.815</v>
       </c>
       <c r="L74">
         <v>0.734</v>
@@ -3871,7 +3871,7 @@
         <v>0.782</v>
       </c>
       <c r="L76">
-        <v>0.68</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="M76">
         <v>0.5629999999999999</v>
@@ -3902,7 +3902,7 @@
         <v>0.887</v>
       </c>
       <c r="G77">
-        <v>0.802</v>
+        <v>0.8020000000000001</v>
       </c>
       <c r="H77">
         <v>0.791</v>
@@ -3942,7 +3942,7 @@
         <v>0.827</v>
       </c>
       <c r="E78">
-        <v>0.801</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="F78">
         <v>0.821</v>
@@ -3960,10 +3960,10 @@
         <v>0.849</v>
       </c>
       <c r="K78">
-        <v>0.805</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="L78">
-        <v>0.68</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="M78">
         <v>0.454</v>
@@ -3988,7 +3988,7 @@
         <v>0.8080000000000001</v>
       </c>
       <c r="E79">
-        <v>0.8139999999999999</v>
+        <v>0.814</v>
       </c>
       <c r="F79">
         <v>0.836</v>
@@ -4031,7 +4031,7 @@
         <v>0.985</v>
       </c>
       <c r="D80">
-        <v>0.931</v>
+        <v>0.9310000000000001</v>
       </c>
       <c r="E80">
         <v>0.872</v>
@@ -4098,7 +4098,7 @@
         <v>0.534</v>
       </c>
       <c r="K81">
-        <v>0.6929999999999999</v>
+        <v>0.693</v>
       </c>
       <c r="L81">
         <v>0.536</v>
@@ -4193,7 +4193,7 @@
         <v>0.57</v>
       </c>
       <c r="L83">
-        <v>0.556</v>
+        <v>0.5560000000000001</v>
       </c>
       <c r="M83">
         <v>0.344</v>
@@ -4399,13 +4399,13 @@
         <v>0.949</v>
       </c>
       <c r="D88">
-        <v>0.926</v>
+        <v>0.9260000000000001</v>
       </c>
       <c r="E88">
         <v>0.9330000000000001</v>
       </c>
       <c r="F88">
-        <v>0.5639999999999999</v>
+        <v>0.564</v>
       </c>
       <c r="G88">
         <v>0.949</v>
@@ -4414,7 +4414,7 @@
         <v>0.973</v>
       </c>
       <c r="I88">
-        <v>0.93</v>
+        <v>0.9300000000000001</v>
       </c>
       <c r="J88">
         <v>0.825</v>
@@ -4506,7 +4506,7 @@
         <v>0.779</v>
       </c>
       <c r="I90">
-        <v>0.8179999999999999</v>
+        <v>0.818</v>
       </c>
       <c r="J90">
         <v>0.772</v>
@@ -4515,7 +4515,7 @@
         <v>0.899</v>
       </c>
       <c r="L90">
-        <v>0.681</v>
+        <v>0.6810000000000001</v>
       </c>
       <c r="M90">
         <v>0.595</v>

</xml_diff>